<commit_message>
fix example workbook InterestRateDerivatives.xlsx so that it calculates correctly on nonworking days - thanks to Paolo Mazzocchi
</commit_message>
<xml_diff>
--- a/QuantLibXL/StandaloneExamples/Analytics/InterestRateDerivatives.xlsx
+++ b/QuantLibXL/StandaloneExamples/Analytics/InterestRateDerivatives.xlsx
@@ -42,6 +42,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -54,6 +55,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -66,6 +68,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -78,6 +81,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>number of days to advance from EvaluationDate (usually zero or two): it fixes the date at which the discount factor = 1.0. If omitted, default = 0 is used.</t>
         </r>
@@ -90,6 +94,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>reference date</t>
         </r>
@@ -102,6 +107,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>cap/floor constant volatility Quote</t>
         </r>
@@ -114,6 +120,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>holiday calendar (e.g. TARGET) to advance from global EvaluationDate</t>
         </r>
@@ -126,6 +133,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>vol quotes</t>
         </r>
@@ -138,6 +146,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>holiday calendar (e.g. TARGET) used for calculating the exercise dates from the expiries</t>
         </r>
@@ -150,6 +159,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>the curve level</t>
         </r>
@@ -162,6 +172,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>DayCounter ID</t>
         </r>
@@ -174,6 +185,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>DayCounter ID</t>
         </r>
@@ -186,6 +198,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>DayCounter ID</t>
         </r>
@@ -198,6 +211,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -210,6 +224,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -222,6 +237,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Interest rate coumpounding rule (Simple:1+rt, Compounded:(1+r)^t, Continuous:e^{rt})</t>
         </r>
@@ -234,6 +250,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -246,6 +263,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -258,6 +276,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>frequency (e.g. Annual, Semiannual, Every4Month, Quarterly, Bimonthly, Monthly). If omitted, default = Annual is used.</t>
         </r>
@@ -270,6 +289,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -282,6 +302,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -304,6 +325,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -316,6 +338,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>effective date</t>
         </r>
@@ -328,6 +351,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>termination date</t>
         </r>
@@ -340,6 +364,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>tenor (e.g. 2D for two days , 3W for three weeks, 6M for six months, 1Y for one year)</t>
         </r>
@@ -352,6 +377,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>holiday calendar (e.g. TARGET)</t>
         </r>
@@ -364,6 +390,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>accrual dates business day convention</t>
         </r>
@@ -376,6 +403,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>termination date business day convention</t>
         </r>
@@ -388,6 +416,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Date generation rule (Backward, Forward, ThirdWednesday, Zero)</t>
         </r>
@@ -400,6 +429,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>end of month convention. FALSE by default.</t>
         </r>
@@ -412,6 +442,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>stub date, if there is an irregular starting period. NA by default.</t>
         </r>
@@ -424,6 +455,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>stub date, if there an irregular final period. NA by default.</t>
         </r>
@@ -436,6 +468,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -448,6 +481,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -460,6 +494,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -472,6 +507,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>effective date</t>
         </r>
@@ -484,6 +520,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>termination date</t>
         </r>
@@ -496,6 +533,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>tenor (e.g. 2D for two days , 3W for three weeks, 6M for six months, 1Y for one year)</t>
         </r>
@@ -508,6 +546,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>holiday calendar (e.g. TARGET)</t>
         </r>
@@ -520,6 +559,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>accrual dates business day convention</t>
         </r>
@@ -532,6 +572,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>termination date business day convention</t>
         </r>
@@ -544,6 +585,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Date generation rule (Backward, Forward, ThirdWednesday, Zero)</t>
         </r>
@@ -556,6 +598,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>end of month convention. FALSE by default.</t>
         </r>
@@ -568,6 +611,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>stub date, if there is an irregular starting period. NA by default.</t>
         </r>
@@ -580,6 +624,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>stub date, if there an irregular final period. NA by default.</t>
         </r>
@@ -592,6 +637,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -604,6 +650,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -626,6 +673,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -638,6 +686,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>discounting yield term structure object ID</t>
         </r>
@@ -650,6 +699,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -662,6 +712,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -674,6 +725,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -686,6 +738,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>discounting yield term structure object ID</t>
         </r>
@@ -698,6 +751,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>OptionletVolatilityStructure object ID</t>
         </r>
@@ -710,6 +764,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -722,6 +777,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -734,6 +790,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -746,6 +803,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>discounting yield term structure object ID</t>
         </r>
@@ -758,6 +816,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>SwaptionVolatilityStructure object ID</t>
         </r>
@@ -770,6 +829,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -782,6 +842,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -804,6 +865,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -816,6 +878,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -828,6 +891,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>index tenor (e.g. 3W for three weeks, 6M for six months, 1Y for one year)</t>
         </r>
@@ -840,6 +904,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>PAYER to pay the fixed rate, RECEIVER to receive it</t>
         </r>
@@ -852,6 +917,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>forecasting yield term structure</t>
         </r>
@@ -864,6 +930,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Notional Amount</t>
         </r>
@@ -876,6 +943,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -888,6 +956,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>fixed leg schedule object ID</t>
         </r>
@@ -900,6 +969,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -912,6 +982,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>the fixed rate</t>
         </r>
@@ -924,6 +995,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>fixed leg day counter (e.g. Actual/360)</t>
         </r>
@@ -936,6 +1008,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating leg schedule object ID</t>
         </r>
@@ -948,6 +1021,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating leg IborIndex object ID</t>
         </r>
@@ -960,6 +1034,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -972,6 +1047,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Index Spread</t>
         </r>
@@ -984,6 +1060,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>payment business day convention. If omitted, default = Following.</t>
         </r>
@@ -996,6 +1073,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating day counter (e.g. Actual/360)</t>
         </r>
@@ -1008,6 +1086,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Nominal amount vector. If omitted, default = 1000000</t>
         </r>
@@ -1020,6 +1099,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1032,6 +1112,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Schedule object ID</t>
         </r>
@@ -1044,6 +1125,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1056,6 +1138,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>fixing days (e.g. 2). If omitted, default = index natural fixing days</t>
         </r>
@@ -1068,6 +1151,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the fixing is in arrears. If omitted, default = FALSE</t>
         </r>
@@ -1080,6 +1164,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Payment DayCounter ID</t>
         </r>
@@ -1092,6 +1177,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floor strikes. If omitted, default = no floor</t>
         </r>
@@ -1104,6 +1190,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1116,6 +1203,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate gearings. If omitted, default = 1.0</t>
         </r>
@@ -1128,6 +1216,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>leg object IDs</t>
         </r>
@@ -1140,6 +1229,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate index</t>
         </r>
@@ -1152,6 +1242,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE for payed leg</t>
         </r>
@@ -1164,6 +1255,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate spreads. If omitted, default = 0%</t>
         </r>
@@ -1176,6 +1268,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1188,6 +1281,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>cap strikes. If omitted, default = no cap</t>
         </r>
@@ -1200,6 +1294,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1212,6 +1307,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1224,6 +1320,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1236,6 +1333,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1248,6 +1346,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>payment business day convention. If omitted, default = Following.</t>
         </r>
@@ -1260,6 +1359,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Nominal amount vector. If omitted, default = 1000000</t>
         </r>
@@ -1272,6 +1372,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Schedule object ID</t>
         </r>
@@ -1284,6 +1385,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>coupon fixed rates</t>
         </r>
@@ -1296,6 +1398,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Payment DayCounter ID</t>
         </r>
@@ -1308,6 +1411,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1320,6 +1424,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1342,6 +1447,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1354,6 +1460,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>option type (cap or floor)</t>
         </r>
@@ -1366,6 +1473,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>coupon vector</t>
         </r>
@@ -1378,6 +1486,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>strikes</t>
         </r>
@@ -1390,6 +1499,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1402,6 +1512,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1414,6 +1525,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1426,6 +1538,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>option type (cap or floor)</t>
         </r>
@@ -1438,6 +1551,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>coupon vector</t>
         </r>
@@ -1450,6 +1564,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>strikes</t>
         </r>
@@ -1462,6 +1577,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1474,6 +1590,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1496,6 +1613,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1508,6 +1626,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>expiry date</t>
         </r>
@@ -1520,6 +1639,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1532,6 +1652,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1544,6 +1665,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1556,6 +1678,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>underlying (vanilla) swap object ID</t>
         </r>
@@ -1568,6 +1691,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Exercise object ID</t>
         </r>
@@ -1580,6 +1704,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>settlement type (PhysicalSettlement, CashSettlement)</t>
         </r>
@@ -1592,6 +1717,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1604,6 +1730,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1626,6 +1753,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1638,6 +1766,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1650,6 +1779,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>index tenor (e.g. 1Y for one year)</t>
         </r>
@@ -1662,6 +1792,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>leg object IDs</t>
         </r>
@@ -1674,6 +1805,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>forecasting yield term structure</t>
         </r>
@@ -1686,6 +1818,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE for payed leg</t>
         </r>
@@ -1698,6 +1831,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1710,6 +1844,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1722,6 +1857,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1734,6 +1870,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1746,6 +1883,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1758,6 +1896,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Swaption Volatility Structure object ID</t>
         </r>
@@ -1770,6 +1909,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Cms Coupon Pricer Type (e.g ConundrumByBlack, ConundrumByNumericalIntegration, ClassicalAnaliticalFormula)</t>
         </r>
@@ -1782,6 +1922,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>model of the yield curve (e.g Standard, ExactYield, ParallelShifts, NonParallelShifts)</t>
         </r>
@@ -1794,6 +1935,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>mean reversion quote.</t>
         </r>
@@ -1806,6 +1948,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1818,6 +1961,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1830,6 +1974,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1842,6 +1987,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>payment business day convention. If omitted, default = Following.</t>
         </r>
@@ -1854,6 +2000,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Nominal amount vector. If omitted, default = 1000000</t>
         </r>
@@ -1866,6 +2013,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Schedule object ID</t>
         </r>
@@ -1878,6 +2026,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>fixing days (e.g. 2). If omitted, default = index natural fixing days</t>
         </r>
@@ -1890,6 +2039,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the fixing is in arrears. If omitted, default = FALSE</t>
         </r>
@@ -1902,6 +2052,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Payment DayCounter ID</t>
         </r>
@@ -1914,6 +2065,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floor strikes. If omitted, default = no floor</t>
         </r>
@@ -1926,6 +2078,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate gearings. If omitted, default = 1.0</t>
         </r>
@@ -1938,6 +2091,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>underlying SwapIndex object ID</t>
         </r>
@@ -1950,6 +2104,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate spreads. If omitted, default = 0%</t>
         </r>
@@ -1962,6 +2117,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>cap strikes. If omitted, default = no cap</t>
         </r>
@@ -1974,6 +2130,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1986,6 +2143,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -2300,10 +2458,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.0000%"/>
-    <numFmt numFmtId="173" formatCode="ddd\,\ d\-mmm\-yyyy"/>
-    <numFmt numFmtId="176" formatCode="0.0000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="ddd\,\ d\-mmm\-yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -2313,11 +2471,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2481,10 +2641,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2503,7 +2663,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2515,9 +2675,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2550,17 +2710,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2572,19 +2732,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2891,7 +3057,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2912,21 +3078,21 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlFlatForward(B3,B4,B5,B6,B7,B8,B9,B10,B11)</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="11" t="str">
         <f>_xll.qlConstantSwaptionVolatility(E3,0,"TARGET","f",E5,E6,E7,E8)</f>
-        <v>obj_00050#0001</v>
+        <v>obj_00004#0016</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>96</v>
       </c>
       <c r="H1" s="11" t="str">
         <f>_xll.qlConstantOptionletVolatility(H3,0,H5,"f",H4,H6,H7,H8)</f>
-        <v>obj_0004d#0001</v>
+        <v>obj_00007#0010</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -2976,7 +3142,7 @@
       </c>
       <c r="E4" s="15">
         <f>_xll.qlSettingsEvaluationDate()</f>
-        <v>41768</v>
+        <v>42097</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>15</v>
@@ -2989,7 +3155,7 @@
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="43" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -3001,7 +3167,7 @@
       <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="43" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3039,7 +3205,7 @@
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -3055,7 +3221,7 @@
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="43" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3194,22 +3360,22 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="34">
-        <v>41956</v>
+        <v>42286</v>
       </c>
       <c r="B2" s="35">
-        <v>22428.645264951807</v>
+        <v>22305.401021215144</v>
       </c>
       <c r="C2" s="35">
         <v>1000000</v>
       </c>
       <c r="D2" s="41">
-        <v>41772</v>
+        <v>42103</v>
       </c>
       <c r="E2" s="41">
-        <v>41956</v>
+        <v>42286</v>
       </c>
       <c r="F2" s="36">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G2" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3218,16 +3384,16 @@
         <v>2</v>
       </c>
       <c r="I2" s="41">
-        <v>41768</v>
+        <v>42101</v>
       </c>
       <c r="J2" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K2" s="38">
-        <v>0.51111111111111107</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L2" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="M2" s="39" t="str">
         <v>#N/A</v>
@@ -3236,7 +3402,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="P2" s="39">
         <v>0</v>
@@ -3278,22 +3444,22 @@
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="34">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="B3" s="35">
-        <v>22058.957099786003</v>
+        <v>22551.90436642418</v>
       </c>
       <c r="C3" s="35">
         <v>1000000</v>
       </c>
       <c r="D3" s="41">
-        <v>41956</v>
+        <v>42286</v>
       </c>
       <c r="E3" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="F3" s="36">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G3" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3302,16 +3468,16 @@
         <v>2</v>
       </c>
       <c r="I3" s="41">
-        <v>41954</v>
+        <v>42284</v>
       </c>
       <c r="J3" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K3" s="38">
-        <v>0.50277777777777777</v>
+        <v>0.51388888888888884</v>
       </c>
       <c r="L3" s="39">
-        <v>4.3874168817253929E-2</v>
+        <v>4.3884786875203814E-2</v>
       </c>
       <c r="M3" s="39" t="str">
         <v>#N/A</v>
@@ -3320,7 +3486,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="39">
-        <v>4.3874168817253929E-2</v>
+        <v>4.3884786875203814E-2</v>
       </c>
       <c r="P3" s="39">
         <v>0</v>
@@ -3362,22 +3528,22 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="34">
-        <v>42321</v>
+        <v>42653</v>
       </c>
       <c r="B4" s="35">
-        <v>22428.645264951811</v>
+        <v>22182.171633423619</v>
       </c>
       <c r="C4" s="35">
         <v>1000000</v>
       </c>
       <c r="D4" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="E4" s="41">
-        <v>42321</v>
+        <v>42653</v>
       </c>
       <c r="F4" s="36">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G4" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3386,16 +3552,16 @@
         <v>2</v>
       </c>
       <c r="I4" s="41">
-        <v>42135</v>
+        <v>42467</v>
       </c>
       <c r="J4" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K4" s="38">
-        <v>0.51111111111111107</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="L4" s="39">
-        <v>4.388213204012311E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="M4" s="39" t="str">
         <v>#N/A</v>
@@ -3404,10 +3570,10 @@
         <v>1</v>
       </c>
       <c r="O4" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="P4" s="39">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="39">
         <v>0</v>
@@ -3446,7 +3612,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="34">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="B5" s="35">
         <v>22182.171633423615</v>
@@ -3455,10 +3621,10 @@
         <v>1000000</v>
       </c>
       <c r="D5" s="41">
-        <v>42321</v>
+        <v>42653</v>
       </c>
       <c r="E5" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="F5" s="36">
         <v>182</v>
@@ -3470,7 +3636,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="41">
-        <v>42319</v>
+        <v>42649</v>
       </c>
       <c r="J5" s="36" t="str">
         <v>Actual/360</v>
@@ -3530,22 +3696,22 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="34">
-        <v>42688</v>
+        <v>43017</v>
       </c>
       <c r="B6" s="35">
-        <v>22551.904366423958</v>
+        <v>22182.171633423615</v>
       </c>
       <c r="C6" s="35">
         <v>1000000</v>
       </c>
       <c r="D6" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="E6" s="41">
-        <v>42688</v>
+        <v>43017</v>
       </c>
       <c r="F6" s="36">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G6" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3554,16 +3720,16 @@
         <v>2</v>
       </c>
       <c r="I6" s="41">
-        <v>42501</v>
+        <v>42831</v>
       </c>
       <c r="J6" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K6" s="38">
-        <v>0.51388888888888884</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="L6" s="39">
-        <v>4.3884786875203384E-2</v>
+        <v>4.3876823011167597E-2</v>
       </c>
       <c r="M6" s="39" t="str">
         <v>#N/A</v>
@@ -3572,10 +3738,10 @@
         <v>1</v>
       </c>
       <c r="O6" s="39">
-        <v>4.3884786875203384E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="P6" s="39">
-        <v>0</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="Q6" s="39">
         <v>0</v>
@@ -3614,7 +3780,7 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="34">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="B7" s="35">
         <v>22182.171633423619</v>
@@ -3623,10 +3789,10 @@
         <v>1000000</v>
       </c>
       <c r="D7" s="41">
-        <v>42688</v>
+        <v>43017</v>
       </c>
       <c r="E7" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="F7" s="36">
         <v>182</v>
@@ -3638,7 +3804,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="41">
-        <v>42684</v>
+        <v>43013</v>
       </c>
       <c r="J7" s="36" t="str">
         <v>Actual/360</v>
@@ -3698,22 +3864,22 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
-        <v>43052</v>
+        <v>43382</v>
       </c>
       <c r="B8" s="35">
-        <v>22182.171633423619</v>
+        <v>22305.401021215366</v>
       </c>
       <c r="C8" s="35">
         <v>1000000</v>
       </c>
       <c r="D8" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="E8" s="41">
-        <v>43052</v>
+        <v>43382</v>
       </c>
       <c r="F8" s="36">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G8" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3722,16 +3888,16 @@
         <v>2</v>
       </c>
       <c r="I8" s="41">
-        <v>42866</v>
+        <v>43195</v>
       </c>
       <c r="J8" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K8" s="38">
-        <v>0.50555555555555554</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L8" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="M8" s="39" t="str">
         <v>#N/A</v>
@@ -3740,7 +3906,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="P8" s="39">
         <v>0</v>
@@ -3782,19 +3948,19 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="B9" s="35">
-        <v>22182.171633423397</v>
+        <v>22182.171633423615</v>
       </c>
       <c r="C9" s="35">
         <v>1000000</v>
       </c>
       <c r="D9" s="41">
-        <v>43052</v>
+        <v>43382</v>
       </c>
       <c r="E9" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="F9" s="36">
         <v>182</v>
@@ -3806,7 +3972,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="41">
-        <v>43048</v>
+        <v>43378</v>
       </c>
       <c r="J9" s="36" t="str">
         <v>Actual/360</v>
@@ -3815,7 +3981,7 @@
         <v>0.50555555555555554</v>
       </c>
       <c r="L9" s="39">
-        <v>4.387682301116716E-2</v>
+        <v>4.3876823011167597E-2</v>
       </c>
       <c r="M9" s="39" t="str">
         <v>#N/A</v>
@@ -3824,10 +3990,10 @@
         <v>1</v>
       </c>
       <c r="O9" s="39">
-        <v>4.387682301116716E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="P9" s="39">
-        <v>0</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="Q9" s="39">
         <v>0</v>
@@ -3866,19 +4032,19 @@
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
-        <v>43417</v>
+        <v>43747</v>
       </c>
       <c r="B10" s="35">
-        <v>22305.40102121537</v>
+        <v>22305.401021215144</v>
       </c>
       <c r="C10" s="35">
         <v>1000000</v>
       </c>
       <c r="D10" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="E10" s="41">
-        <v>43417</v>
+        <v>43747</v>
       </c>
       <c r="F10" s="36">
         <v>183</v>
@@ -3890,7 +4056,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="41">
-        <v>43230</v>
+        <v>43560</v>
       </c>
       <c r="J10" s="36" t="str">
         <v>Actual/360</v>
@@ -3899,7 +4065,7 @@
         <v>0.5083333333333333</v>
       </c>
       <c r="L10" s="39">
-        <v>4.3879477418784334E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="M10" s="39" t="str">
         <v>#N/A</v>
@@ -3908,10 +4074,10 @@
         <v>1</v>
       </c>
       <c r="O10" s="39">
-        <v>4.3879477418784327E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="P10" s="39">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="39">
         <v>0</v>
@@ -3950,22 +4116,22 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="B11" s="35">
-        <v>22058.957099786003</v>
+        <v>22305.401021215144</v>
       </c>
       <c r="C11" s="35">
         <v>1000000</v>
       </c>
       <c r="D11" s="41">
-        <v>43417</v>
+        <v>43747</v>
       </c>
       <c r="E11" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="F11" s="36">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G11" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3974,16 +4140,16 @@
         <v>2</v>
       </c>
       <c r="I11" s="41">
-        <v>43413</v>
+        <v>43745</v>
       </c>
       <c r="J11" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K11" s="38">
-        <v>0.50277777777777777</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L11" s="39">
-        <v>4.3874168817253929E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="M11" s="39" t="str">
         <v>#N/A</v>
@@ -3992,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="39">
-        <v>4.3874168817253929E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="P11" s="39">
         <v>0</v>
@@ -4034,22 +4200,22 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="34">
-        <v>43782</v>
+        <v>44113</v>
       </c>
       <c r="B12" s="35">
-        <v>22428.645264951807</v>
+        <v>22305.40102121537</v>
       </c>
       <c r="C12" s="35">
         <v>1000000</v>
       </c>
       <c r="D12" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="E12" s="41">
-        <v>43782</v>
+        <v>44113</v>
       </c>
       <c r="F12" s="36">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G12" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4058,16 +4224,16 @@
         <v>2</v>
       </c>
       <c r="I12" s="41">
-        <v>43594</v>
+        <v>43928</v>
       </c>
       <c r="J12" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K12" s="38">
-        <v>0.51111111111111107</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L12" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3879477418784334E-2</v>
       </c>
       <c r="M12" s="39" t="str">
         <v>#N/A</v>
@@ -4076,10 +4242,10 @@
         <v>1</v>
       </c>
       <c r="O12" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="P12" s="39">
-        <v>0</v>
+        <v>6.9388939039072284E-18</v>
       </c>
       <c r="Q12" s="39">
         <v>0</v>
@@ -4118,7 +4284,7 @@
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="34">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="B13" s="35">
         <v>22182.171633423615</v>
@@ -4127,10 +4293,10 @@
         <v>1000000</v>
       </c>
       <c r="D13" s="41">
-        <v>43782</v>
+        <v>44113</v>
       </c>
       <c r="E13" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="F13" s="36">
         <v>182</v>
@@ -4142,7 +4308,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="41">
-        <v>43780</v>
+        <v>44111</v>
       </c>
       <c r="J13" s="36" t="str">
         <v>Actual/360</v>
@@ -4202,22 +4368,22 @@
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="34">
-        <v>44148</v>
+        <v>44480</v>
       </c>
       <c r="B14" s="35">
-        <v>22428.645264951807</v>
+        <v>22551.90436642418</v>
       </c>
       <c r="C14" s="35">
         <v>1000000</v>
       </c>
       <c r="D14" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="E14" s="41">
-        <v>44148</v>
+        <v>44480</v>
       </c>
       <c r="F14" s="36">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G14" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4226,16 +4392,16 @@
         <v>2</v>
       </c>
       <c r="I14" s="41">
-        <v>43962</v>
+        <v>44293</v>
       </c>
       <c r="J14" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K14" s="38">
-        <v>0.51111111111111107</v>
+        <v>0.51388888888888884</v>
       </c>
       <c r="L14" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3884786875203814E-2</v>
       </c>
       <c r="M14" s="39" t="str">
         <v>#N/A</v>
@@ -4244,7 +4410,7 @@
         <v>1</v>
       </c>
       <c r="O14" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3884786875203814E-2</v>
       </c>
       <c r="P14" s="39">
         <v>0</v>
@@ -4286,22 +4452,22 @@
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="34">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="B15" s="35">
-        <v>22058.957099786221</v>
+        <v>22182.171633423619</v>
       </c>
       <c r="C15" s="35">
         <v>1000000</v>
       </c>
       <c r="D15" s="41">
-        <v>44148</v>
+        <v>44480</v>
       </c>
       <c r="E15" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="F15" s="36">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G15" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4310,16 +4476,16 @@
         <v>2</v>
       </c>
       <c r="I15" s="41">
-        <v>44146</v>
+        <v>44476</v>
       </c>
       <c r="J15" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K15" s="38">
-        <v>0.50277777777777777</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="L15" s="39">
-        <v>4.3874168817254366E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="M15" s="39" t="str">
         <v>#N/A</v>
@@ -4328,10 +4494,10 @@
         <v>1</v>
       </c>
       <c r="O15" s="39">
-        <v>4.3874168817254373E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="P15" s="39">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="39">
         <v>0</v>
@@ -4370,22 +4536,22 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="34">
-        <v>44515</v>
+        <v>44844</v>
       </c>
       <c r="B16" s="35">
-        <v>22675.178327423273</v>
+        <v>22182.171633423397</v>
       </c>
       <c r="C16" s="35">
         <v>1000000</v>
       </c>
       <c r="D16" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="E16" s="41">
-        <v>44515</v>
+        <v>44844</v>
       </c>
       <c r="F16" s="36">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G16" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4394,16 +4560,16 @@
         <v>2</v>
       </c>
       <c r="I16" s="41">
-        <v>44327</v>
+        <v>44658</v>
       </c>
       <c r="J16" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K16" s="38">
-        <v>0.51666666666666672</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="L16" s="39">
-        <v>4.3887441924045041E-2</v>
+        <v>4.387682301116716E-2</v>
       </c>
       <c r="M16" s="39" t="str">
         <v>#N/A</v>
@@ -4412,7 +4578,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="39">
-        <v>4.3887441924045041E-2</v>
+        <v>4.387682301116716E-2</v>
       </c>
       <c r="P16" s="39">
         <v>0</v>
@@ -4454,22 +4620,22 @@
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="34">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="B17" s="35">
-        <v>21812.572587811996</v>
+        <v>22305.401021215366</v>
       </c>
       <c r="C17" s="35">
         <v>1000000</v>
       </c>
       <c r="D17" s="41">
-        <v>44515</v>
+        <v>44844</v>
       </c>
       <c r="E17" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="F17" s="36">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G17" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4478,16 +4644,16 @@
         <v>2</v>
       </c>
       <c r="I17" s="41">
-        <v>44511</v>
+        <v>44840</v>
       </c>
       <c r="J17" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K17" s="38">
-        <v>0.49722222222222223</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L17" s="39">
-        <v>4.3868861070459876E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="M17" s="39" t="str">
         <v>#N/A</v>
@@ -4496,7 +4662,7 @@
         <v>1</v>
       </c>
       <c r="O17" s="39">
-        <v>4.3868861070459876E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="P17" s="39">
         <v>0</v>
@@ -4538,22 +4704,22 @@
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="34">
-        <v>44879</v>
+        <v>45208</v>
       </c>
       <c r="B18" s="35">
-        <v>22551.904366423954</v>
+        <v>22058.957099786221</v>
       </c>
       <c r="C18" s="35">
         <v>1000000</v>
       </c>
       <c r="D18" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="E18" s="41">
-        <v>44879</v>
+        <v>45208</v>
       </c>
       <c r="F18" s="36">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G18" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4562,16 +4728,16 @@
         <v>2</v>
       </c>
       <c r="I18" s="41">
-        <v>44692</v>
+        <v>45021</v>
       </c>
       <c r="J18" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K18" s="38">
-        <v>0.51388888888888884</v>
+        <v>0.50277777777777777</v>
       </c>
       <c r="L18" s="39">
-        <v>4.3884786875203377E-2</v>
+        <v>4.3874168817254366E-2</v>
       </c>
       <c r="M18" s="39" t="str">
         <v>#N/A</v>
@@ -4580,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="O18" s="39">
-        <v>4.3884786875203384E-2</v>
+        <v>4.3874168817254373E-2</v>
       </c>
       <c r="P18" s="39">
         <v>-6.9388939039072284E-18</v>
@@ -4622,22 +4788,22 @@
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="34">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="B19" s="35">
-        <v>22182.171633423619</v>
+        <v>22305.401021215366</v>
       </c>
       <c r="C19" s="35">
         <v>1000000</v>
       </c>
       <c r="D19" s="41">
-        <v>44879</v>
+        <v>45208</v>
       </c>
       <c r="E19" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="F19" s="36">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G19" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4646,16 +4812,16 @@
         <v>2</v>
       </c>
       <c r="I19" s="41">
-        <v>44875</v>
+        <v>45204</v>
       </c>
       <c r="J19" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K19" s="38">
-        <v>0.50555555555555554</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L19" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="M19" s="39" t="str">
         <v>#N/A</v>
@@ -4664,7 +4830,7 @@
         <v>1</v>
       </c>
       <c r="O19" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="P19" s="39">
         <v>0</v>
@@ -4706,22 +4872,22 @@
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="34">
-        <v>45243</v>
+        <v>45574</v>
       </c>
       <c r="B20" s="35">
-        <v>22182.171633423615</v>
+        <v>22305.401021214922</v>
       </c>
       <c r="C20" s="35">
         <v>1000000</v>
       </c>
       <c r="D20" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="E20" s="41">
-        <v>45243</v>
+        <v>45574</v>
       </c>
       <c r="F20" s="36">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G20" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4730,16 +4896,16 @@
         <v>2</v>
       </c>
       <c r="I20" s="41">
-        <v>45057</v>
+        <v>45387</v>
       </c>
       <c r="J20" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K20" s="38">
-        <v>0.50555555555555554</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L20" s="39">
-        <v>4.3876823011167597E-2</v>
+        <v>4.3879477418783452E-2</v>
       </c>
       <c r="M20" s="39" t="str">
         <v>#N/A</v>
@@ -4748,10 +4914,10 @@
         <v>1</v>
       </c>
       <c r="O20" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418783452E-2</v>
       </c>
       <c r="P20" s="39">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="39">
         <v>0</v>
@@ -4790,19 +4956,19 @@
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="34">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="B21" s="35">
-        <v>22182.171633423401</v>
+        <v>22182.171633423841</v>
       </c>
       <c r="C21" s="35">
         <v>1000000</v>
       </c>
       <c r="D21" s="41">
-        <v>45243</v>
+        <v>45574</v>
       </c>
       <c r="E21" s="41">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="F21" s="36">
         <v>182</v>
@@ -4814,7 +4980,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="41">
-        <v>45239</v>
+        <v>45572</v>
       </c>
       <c r="J21" s="36" t="str">
         <v>Actual/360</v>
@@ -4823,7 +4989,7 @@
         <v>0.50555555555555554</v>
       </c>
       <c r="L21" s="39">
-        <v>4.3876823011167167E-2</v>
+        <v>4.3876823011168041E-2</v>
       </c>
       <c r="M21" s="39" t="str">
         <v>#N/A</v>
@@ -4832,10 +4998,10 @@
         <v>1</v>
       </c>
       <c r="O21" s="39">
-        <v>4.387682301116716E-2</v>
+        <v>4.3876823011168041E-2</v>
       </c>
       <c r="P21" s="39">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="39">
         <v>0</v>
@@ -5179,7 +5345,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5195,7 +5361,7 @@
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="44" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5204,8 +5370,8 @@
         <v>35</v>
       </c>
       <c r="B2" s="15">
-        <f>_xll.qlCalendarAdvance(Calendar,ReferenceDate,"2d")</f>
-        <v>41772</v>
+        <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdjust(Calendar,ReferenceDate,"f"),"2d")</f>
+        <v>42103</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5214,7 +5380,7 @@
       </c>
       <c r="B3" s="29">
         <f>_xll.qlCalendarAdvance(Calendar,B2,"10Y","Unadjusted")</f>
-        <v>45425</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -5224,7 +5390,7 @@
       </c>
       <c r="B5" s="11" t="str">
         <f>_xll.qlSchedule(B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19)</f>
-        <v>obj_00051#0001</v>
+        <v>obj_00009#0013</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5248,7 +5414,7 @@
       </c>
       <c r="B8" s="15">
         <f>EffectiveDate</f>
-        <v>41772</v>
+        <v>42103</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -5257,7 +5423,7 @@
       </c>
       <c r="B9" s="15">
         <f>TerminationDate</f>
-        <v>45425</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -5337,7 +5503,7 @@
       </c>
       <c r="B21" s="11" t="str">
         <f>_xll.qlSchedule(B23,B24,B25,B26,B27,B28,B29,B30,B31,B32,B33,B34,B35)</f>
-        <v>obj_00052#0001</v>
+        <v>obj_0000a#0013</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5361,7 +5527,7 @@
       </c>
       <c r="B24" s="15">
         <f>EffectiveDate</f>
-        <v>41772</v>
+        <v>42103</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -5370,7 +5536,7 @@
       </c>
       <c r="B25" s="15">
         <f>TerminationDate</f>
-        <v>45425</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -5465,7 +5631,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5480,7 +5646,7 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlDiscountingSwapEngine(B3,B4,B5,B6)</f>
-        <v>obj_00054#0001</v>
+        <v>obj_00001#0020</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5504,7 +5670,7 @@
       </c>
       <c r="B4" s="8" t="str">
         <f>TermStructures!$B$1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -5526,7 +5692,7 @@
       </c>
       <c r="B8" s="11" t="str">
         <f>_xll.qlBlackCapFloorEngine(B10,B11,B12,B13,B14)</f>
-        <v>obj_00057#0001</v>
+        <v>obj_00008#0021</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5550,7 +5716,7 @@
       </c>
       <c r="B11" s="8" t="str">
         <f>TermStructures!$B$1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5559,7 +5725,7 @@
       </c>
       <c r="B12" s="8" t="str">
         <f>TermStructures!$H$1</f>
-        <v>obj_0004d#0001</v>
+        <v>obj_00007#0010</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -5581,7 +5747,7 @@
       </c>
       <c r="B16" s="11" t="str">
         <f>_xll.qlBlackSwaptionEngine(B18,B19,B20,B21,B22)</f>
-        <v>obj_00055#0001</v>
+        <v>obj_00006#0021</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5605,7 +5771,7 @@
       </c>
       <c r="B19" s="8" t="str">
         <f>TermStructures!$B$1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -5614,7 +5780,7 @@
       </c>
       <c r="B20" s="8" t="str">
         <f>TermStructures!$E$1</f>
-        <v>obj_00050#0001</v>
+        <v>obj_00004#0016</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -5643,7 +5809,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5665,14 +5831,14 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlEuribor(B3,B4,B5,B6,B7)</f>
-        <v>obj_00058#0001</v>
+        <v>obj_00003#0024</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="11" t="str">
         <f>_xll.qlVanillaSwap(E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14)</f>
-        <v>obj_0005c#0001</v>
+        <v>obj_0000c#0028</v>
       </c>
       <c r="H1" t="s">
         <v>75</v>
@@ -5702,7 +5868,7 @@
       </c>
       <c r="I2" s="27">
         <f>_xll.qlInstrumentNPV(E1,I1)</f>
-        <v>-39387.492820908315</v>
+        <v>-39363.257108460588</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5719,7 +5885,7 @@
       </c>
       <c r="I3" s="28">
         <f>_xll.qlVanillaSwapFairRate($E$1,$I$1)</f>
-        <v>4.5019439201856769E-2</v>
+        <v>4.5021117962698143E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5741,7 +5907,7 @@
       </c>
       <c r="I4" s="28">
         <f>_xll.qlVanillaSwapFairSpread($E$1,$I$1)</f>
-        <v>4.8543530153119544E-3</v>
+        <v>4.8525326129049808E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5750,7 +5916,7 @@
       </c>
       <c r="B5" s="8" t="str">
         <f>TermStructures!B1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>23</v>
@@ -5770,7 +5936,7 @@
       </c>
       <c r="E6" s="8" t="str">
         <f>DateCalc!$B$5</f>
-        <v>obj_00051#0001</v>
+        <v>obj_00009#0013</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5801,14 +5967,14 @@
       </c>
       <c r="B9" s="11" t="str">
         <f>_xll.qlIborLeg(B11,B12,B13,B14,B15,B16,B17,B18,B19,B20,B21,B22,B23,B24)</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="8" t="str">
         <f>DateCalc!B21</f>
-        <v>obj_00052#0001</v>
+        <v>obj_0000a#0013</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5824,7 +5990,7 @@
       </c>
       <c r="E10" s="8" t="str">
         <f>B1</f>
-        <v>obj_00058#0001</v>
+        <v>obj_00003#0024</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5873,7 +6039,7 @@
       </c>
       <c r="B14" s="8" t="str">
         <f>DateCalc!B21</f>
-        <v>obj_00052#0001</v>
+        <v>obj_0000a#0013</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>11</v>
@@ -5896,7 +6062,7 @@
       </c>
       <c r="E16" s="11" t="str">
         <f>_xll.qlSwap(E18,E19:F19,E20:F20,E21,E22)</f>
-        <v>obj_00060#0001</v>
+        <v>obj_00010#0020</v>
       </c>
       <c r="H16" t="s">
         <v>75</v>
@@ -5925,7 +6091,7 @@
       </c>
       <c r="I17" s="27">
         <f>_xll.qlInstrumentNPV(E16,I16)</f>
-        <v>-39387.492820908315</v>
+        <v>-39363.257108460588</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5949,11 +6115,11 @@
       </c>
       <c r="E19" s="17" t="str">
         <f>B26</f>
-        <v>obj_0005b#0001</v>
+        <v>obj_0000b#0013</v>
       </c>
       <c r="F19" s="18" t="str">
         <f>B9</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5962,7 +6128,7 @@
       </c>
       <c r="B20" s="8" t="str">
         <f>B1</f>
-        <v>obj_00058#0001</v>
+        <v>obj_00003#0024</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>18</v>
@@ -6013,7 +6179,7 @@
       </c>
       <c r="B26" s="11" t="str">
         <f>_xll.qlFixedRateLeg(B28,B29,B30,B31,B32,B33,B34,B35)</f>
-        <v>obj_0005b#0001</v>
+        <v>obj_0000b#0013</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6054,7 +6220,7 @@
       </c>
       <c r="B31" s="8" t="str">
         <f>DateCalc!$B$5</f>
-        <v>obj_00051#0001</v>
+        <v>obj_00009#0013</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -6087,7 +6253,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
       <formula1>"Payer,Receiver"</formula1>
     </dataValidation>
@@ -6128,7 +6294,7 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlCapFloor(B3,B4,B5,B6,B7,B8)</f>
-        <v>obj_0005f#0001</v>
+        <v>obj_00012#0020</v>
       </c>
       <c r="D1" t="s">
         <v>75</v>
@@ -6151,7 +6317,7 @@
       </c>
       <c r="E2" s="27">
         <f>_xll.qlInstrumentNPV(B1,E1)</f>
-        <v>26215.851935305589</v>
+        <v>26175.177192398387</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -6164,7 +6330,7 @@
       </c>
       <c r="E3" s="2">
         <f>_xll.qlCapFloorAtmRate(B1,TermStructures!$B$1)</f>
-        <v>4.3878643248097524E-2</v>
+        <v>4.3878614023525997E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -6188,7 +6354,7 @@
       </c>
       <c r="B5" s="8" t="str">
         <f>Swaps!B9</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -6218,7 +6384,7 @@
       </c>
       <c r="B10" s="11" t="str">
         <f>_xll.qlCapFloor(B12,B13,B14,B15,B16,B17)</f>
-        <v>obj_0005e#0001</v>
+        <v>obj_0000f#0020</v>
       </c>
       <c r="D10" t="s">
         <v>75</v>
@@ -6241,7 +6407,7 @@
       </c>
       <c r="E11" s="27">
         <f>_xll.qlInstrumentNPV(B10,E10)</f>
-        <v>57686.58193937147</v>
+        <v>57638.1045360512</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -6254,7 +6420,7 @@
       </c>
       <c r="E12" s="2">
         <f>_xll.qlCapFloorAtmRate(B10,TermStructures!$B$1)</f>
-        <v>4.3878643248097524E-2</v>
+        <v>4.3878614023525997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -6278,7 +6444,7 @@
       </c>
       <c r="B14" s="8" t="str">
         <f>Swaps!B9</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -6337,7 +6503,7 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlEuropeanExercise(B3,B4,B5,B6)</f>
-        <v>obj_0004e#0001</v>
+        <v>obj_00013#0005</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6382,7 +6548,7 @@
       </c>
       <c r="B8" s="11" t="str">
         <f>_xll.qlSwaption(B10,B11,B12,B13,B14,B15)</f>
-        <v>obj_0005d#0001</v>
+        <v>obj_00014#0018</v>
       </c>
       <c r="D8" t="s">
         <v>75</v>
@@ -6405,7 +6571,7 @@
       </c>
       <c r="E9" s="27">
         <f>_xll.qlInstrumentNPV(B8,E8)</f>
-        <v>8034.9988082185755</v>
+        <v>7964.1828023073604</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -6427,7 +6593,7 @@
       </c>
       <c r="B11" s="8" t="str">
         <f>Swaps!E1</f>
-        <v>obj_0005c#0001</v>
+        <v>obj_0000c#0028</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -6436,7 +6602,7 @@
       </c>
       <c r="B12" s="8" t="str">
         <f>B1</f>
-        <v>obj_0004e#0001</v>
+        <v>obj_00013#0005</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -6499,14 +6665,14 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlEuriborSwapIsdaFixA(B3,B4,B5,B6,B7,B8)</f>
-        <v>obj_00056#0001</v>
+        <v>obj_00002#0020</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E1" s="11" t="str">
         <f>_xll.qlSwap(E3,E4:F4,E5:F5,E6,E7)</f>
-        <v>obj_00061#0001</v>
+        <v>obj_00011#0020</v>
       </c>
       <c r="H1" t="s">
         <v>75</v>
@@ -6536,7 +6702,7 @@
       </c>
       <c r="I2" s="27">
         <f>_xll.qlInstrumentNPV(E1,I1)</f>
-        <v>-11903.469893039088</v>
+        <v>-11879.445724761754</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6562,11 +6728,11 @@
       </c>
       <c r="E4" s="17" t="str">
         <f>B20</f>
-        <v>obj_0005a#0001</v>
+        <v>obj_0000e#0019</v>
       </c>
       <c r="F4" s="18" t="str">
         <f>Swaps!B9</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6575,7 +6741,7 @@
       </c>
       <c r="B5" s="8" t="str">
         <f>TermStructures!B1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>18</v>
@@ -6593,7 +6759,7 @@
       </c>
       <c r="B6" s="8" t="str">
         <f>TermStructures!B1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>10</v>
@@ -6623,7 +6789,7 @@
       </c>
       <c r="B10" s="11" t="str">
         <f>_xll.qlCmsCouponPricer(B12,B13,B14,B15,B16,B17,B18)</f>
-        <v>obj_00053#0001</v>
+        <v>obj_00005#0010</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6647,7 +6813,7 @@
       </c>
       <c r="B13" s="8" t="str">
         <f>TermStructures!E1</f>
-        <v>obj_00050#0001</v>
+        <v>obj_00004#0016</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -6693,7 +6859,7 @@
       </c>
       <c r="B20" s="11" t="str">
         <f>_xll.qlCmsLeg(B22,B23,B24,B25,B26,B27,B28,B29,B30,B31,B32,B33,B34,B35)</f>
-        <v>obj_0005a#0001</v>
+        <v>obj_0000e#0019</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6734,7 +6900,7 @@
       </c>
       <c r="B25" s="8" t="str">
         <f>DateCalc!B5</f>
-        <v>obj_00051#0001</v>
+        <v>obj_00009#0013</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -6775,7 +6941,7 @@
       </c>
       <c r="B31" s="8" t="str">
         <f>B1</f>
-        <v>obj_00056#0001</v>
+        <v>obj_00002#0020</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -6931,22 +7097,22 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="34">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="B2" s="35">
-        <v>50000.000000000044</v>
+        <v>50277.777777777868</v>
       </c>
       <c r="C2" s="35">
         <v>1000000</v>
       </c>
       <c r="D2" s="41">
-        <v>41772</v>
+        <v>42103</v>
       </c>
       <c r="E2" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="F2" s="36">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G2" s="37" t="str">
         <v>#N/A</v>
@@ -6961,7 +7127,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K2" s="38">
-        <v>1</v>
+        <v>1.0055555555555555</v>
       </c>
       <c r="L2" s="39">
         <v>0.05</v>
@@ -7015,22 +7181,22 @@
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="34">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="B3" s="35">
-        <v>50000.000000000044</v>
+        <v>49861.111111111131</v>
       </c>
       <c r="C3" s="35">
         <v>1000000</v>
       </c>
       <c r="D3" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="E3" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="F3" s="36">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G3" s="37" t="str">
         <v>#N/A</v>
@@ -7045,7 +7211,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K3" s="38">
-        <v>1</v>
+        <v>0.99722222222222223</v>
       </c>
       <c r="L3" s="39">
         <v>0.05</v>
@@ -7099,22 +7265,22 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="34">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="B4" s="35">
-        <v>50277.777777777868</v>
+        <v>49861.111111111131</v>
       </c>
       <c r="C4" s="35">
         <v>1000000</v>
       </c>
       <c r="D4" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="E4" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="F4" s="36">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G4" s="37" t="str">
         <v>#N/A</v>
@@ -7129,7 +7295,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K4" s="38">
-        <v>1.0055555555555555</v>
+        <v>0.99722222222222223</v>
       </c>
       <c r="L4" s="39">
         <v>0.05</v>
@@ -7183,22 +7349,22 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="34">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="B5" s="35">
-        <v>49861.111111111131</v>
+        <v>50000.000000000044</v>
       </c>
       <c r="C5" s="35">
         <v>1000000</v>
       </c>
       <c r="D5" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="E5" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="F5" s="36">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G5" s="37" t="str">
         <v>#N/A</v>
@@ -7213,7 +7379,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K5" s="38">
-        <v>0.99722222222222223</v>
+        <v>1</v>
       </c>
       <c r="L5" s="39">
         <v>0.05</v>
@@ -7267,22 +7433,22 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="34">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="B6" s="35">
-        <v>49861.111111111131</v>
+        <v>50000.000000000044</v>
       </c>
       <c r="C6" s="35">
         <v>1000000</v>
       </c>
       <c r="D6" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="E6" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="F6" s="36">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G6" s="37" t="str">
         <v>#N/A</v>
@@ -7297,7 +7463,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K6" s="38">
-        <v>0.99722222222222223</v>
+        <v>1</v>
       </c>
       <c r="L6" s="39">
         <v>0.05</v>
@@ -7351,7 +7517,7 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="34">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="B7" s="35">
         <v>50000.000000000044</v>
@@ -7360,10 +7526,10 @@
         <v>1000000</v>
       </c>
       <c r="D7" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="E7" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="F7" s="36">
         <v>360</v>
@@ -7435,22 +7601,22 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="B8" s="35">
-        <v>50000.000000000044</v>
+        <v>50277.777777777868</v>
       </c>
       <c r="C8" s="35">
         <v>1000000</v>
       </c>
       <c r="D8" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="E8" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="F8" s="36">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G8" s="37" t="str">
         <v>#N/A</v>
@@ -7465,7 +7631,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K8" s="38">
-        <v>1</v>
+        <v>1.0055555555555555</v>
       </c>
       <c r="L8" s="39">
         <v>0.05</v>
@@ -7519,7 +7685,7 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="B9" s="35">
         <v>50000.000000000044</v>
@@ -7528,10 +7694,10 @@
         <v>1000000</v>
       </c>
       <c r="D9" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="E9" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="F9" s="36">
         <v>360</v>
@@ -7603,22 +7769,22 @@
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="B10" s="35">
-        <v>50277.777777777868</v>
+        <v>49722.222222222226</v>
       </c>
       <c r="C10" s="35">
         <v>1000000</v>
       </c>
       <c r="D10" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="E10" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="F10" s="36">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G10" s="37" t="str">
         <v>#N/A</v>
@@ -7633,7 +7799,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K10" s="38">
-        <v>1.0055555555555555</v>
+        <v>0.99444444444444446</v>
       </c>
       <c r="L10" s="39">
         <v>0.05</v>
@@ -7687,22 +7853,22 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="B11" s="35">
-        <v>49722.222222222226</v>
+        <v>50000.000000000044</v>
       </c>
       <c r="C11" s="35">
         <v>1000000</v>
       </c>
       <c r="D11" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="E11" s="41">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="F11" s="36">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G11" s="37" t="str">
         <v>#N/A</v>
@@ -7717,7 +7883,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K11" s="38">
-        <v>0.99444444444444446</v>
+        <v>1</v>
       </c>
       <c r="L11" s="39">
         <v>0.05</v>
@@ -8920,7 +9086,7 @@
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
@@ -8932,9 +9098,7 @@
     <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.83203125" bestFit="1" customWidth="1"/>
@@ -9009,22 +9173,22 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="34">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="B2" s="35">
-        <v>45644.709190771478</v>
+        <v>46021.587250758144</v>
       </c>
       <c r="C2" s="35">
         <v>1000000</v>
       </c>
       <c r="D2" s="41">
-        <v>41772</v>
+        <v>42103</v>
       </c>
       <c r="E2" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="F2" s="36">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="G2" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9033,16 +9197,16 @@
         <v>2</v>
       </c>
       <c r="I2" s="41">
-        <v>41768</v>
+        <v>42101</v>
       </c>
       <c r="J2" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K2" s="38">
-        <v>1.0138888888888888</v>
+        <v>1.0222222222222221</v>
       </c>
       <c r="L2" s="39">
-        <v>4.5019439201856803E-2</v>
+        <v>4.5021117962698191E-2</v>
       </c>
       <c r="M2" s="39" t="str">
         <v>#N/A</v>
@@ -9051,7 +9215,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="39">
-        <v>4.5019439201856803E-2</v>
+        <v>4.5021117962698191E-2</v>
       </c>
       <c r="P2" s="39">
         <v>0</v>
@@ -9074,22 +9238,22 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="34">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="B3" s="35">
-        <v>45965.940727128131</v>
+        <v>45700.234002910169</v>
       </c>
       <c r="C3" s="35">
         <v>1000000</v>
       </c>
       <c r="D3" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="E3" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="F3" s="36">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G3" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9098,16 +9262,16 @@
         <v>2</v>
       </c>
       <c r="I3" s="41">
-        <v>42135</v>
+        <v>42467</v>
       </c>
       <c r="J3" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K3" s="38">
-        <v>1.0166666666666666</v>
+        <v>1.0111111111111111</v>
       </c>
       <c r="L3" s="39">
-        <v>4.5212400715208004E-2</v>
+        <v>4.5198033629251823E-2</v>
       </c>
       <c r="M3" s="39" t="str">
         <v>#N/A</v>
@@ -9116,10 +9280,10 @@
         <v>1</v>
       </c>
       <c r="O3" s="39">
-        <v>4.502110877876498E-2</v>
+        <v>4.5007086676381654E-2</v>
       </c>
       <c r="P3" s="39">
-        <v>1.912919364430235E-4</v>
+        <v>1.9094695287016905E-4</v>
       </c>
       <c r="Q3" s="39">
         <v>0</v>
@@ -9139,22 +9303,22 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="34">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="B4" s="35">
-        <v>46275.038644473956</v>
+        <v>45897.754769535633</v>
       </c>
       <c r="C4" s="35">
         <v>1000000</v>
       </c>
       <c r="D4" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="E4" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="F4" s="36">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G4" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9163,16 +9327,16 @@
         <v>2</v>
       </c>
       <c r="I4" s="41">
-        <v>42501</v>
+        <v>42831</v>
       </c>
       <c r="J4" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K4" s="38">
-        <v>1.0194444444444444</v>
+        <v>1.0111111111111111</v>
       </c>
       <c r="L4" s="39">
-        <v>4.5392408479592986E-2</v>
+        <v>4.5393383838002281E-2</v>
       </c>
       <c r="M4" s="39" t="str">
         <v>#N/A</v>
@@ -9181,10 +9345,10 @@
         <v>1</v>
       </c>
       <c r="O4" s="39">
-        <v>4.5006931640100688E-2</v>
+        <v>4.5008215591537871E-2</v>
       </c>
       <c r="P4" s="39">
-        <v>3.8547683949229777E-4</v>
+        <v>3.8516824646440961E-4</v>
       </c>
       <c r="Q4" s="39">
         <v>0</v>
@@ -9204,22 +9368,22 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="34">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="B5" s="35">
-        <v>46100.705678090198</v>
+        <v>46236.176220051486</v>
       </c>
       <c r="C5" s="35">
         <v>1000000</v>
       </c>
       <c r="D5" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="E5" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="F5" s="36">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G5" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9228,16 +9392,16 @@
         <v>2</v>
       </c>
       <c r="I5" s="41">
-        <v>42866</v>
+        <v>43195</v>
       </c>
       <c r="J5" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K5" s="38">
-        <v>1.0111111111111111</v>
+        <v>1.0138888888888888</v>
       </c>
       <c r="L5" s="39">
-        <v>4.5594104516792508E-2</v>
+        <v>4.5602803943064485E-2</v>
       </c>
       <c r="M5" s="39" t="str">
         <v>#N/A</v>
@@ -9246,10 +9410,10 @@
         <v>1</v>
       </c>
       <c r="O5" s="39">
-        <v>4.5008179983093845E-2</v>
+        <v>4.5019506828358764E-2</v>
       </c>
       <c r="P5" s="39">
-        <v>5.8592453369866321E-4</v>
+        <v>5.832971147057206E-4</v>
       </c>
       <c r="Q5" s="39">
         <v>0</v>
@@ -9269,22 +9433,22 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="34">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="B6" s="35">
-        <v>46317.59147018251</v>
+        <v>46571.044146595494</v>
       </c>
       <c r="C6" s="35">
         <v>1000000</v>
       </c>
       <c r="D6" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="E6" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="F6" s="36">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="G6" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9293,16 +9457,16 @@
         <v>2</v>
       </c>
       <c r="I6" s="41">
-        <v>43230</v>
+        <v>43560</v>
       </c>
       <c r="J6" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K6" s="38">
-        <v>1.0111111111111111</v>
+        <v>1.0166666666666666</v>
       </c>
       <c r="L6" s="39">
-        <v>4.580860694853215E-2</v>
+        <v>4.580758440648737E-2</v>
       </c>
       <c r="M6" s="39" t="str">
         <v>#N/A</v>
@@ -9311,10 +9475,10 @@
         <v>1</v>
       </c>
       <c r="O6" s="39">
-        <v>4.5019502408633533E-2</v>
+        <v>4.5021105506382955E-2</v>
       </c>
       <c r="P6" s="39">
-        <v>7.8910453989861767E-4</v>
+        <v>7.8647890010441479E-4</v>
       </c>
       <c r="Q6" s="39">
         <v>0</v>
@@ -9334,22 +9498,22 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="34">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="B7" s="35">
-        <v>46783.905135645306</v>
+        <v>46641.337224146693</v>
       </c>
       <c r="C7" s="35">
         <v>1000000</v>
       </c>
       <c r="D7" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="E7" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="F7" s="36">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G7" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9358,16 +9522,16 @@
         <v>2</v>
       </c>
       <c r="I7" s="41">
-        <v>43594</v>
+        <v>43928</v>
       </c>
       <c r="J7" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K7" s="38">
-        <v>1.0166666666666666</v>
+        <v>1.0138888888888888</v>
       </c>
       <c r="L7" s="39">
-        <v>4.6016955871126537E-2</v>
+        <v>4.6002414796418659E-2</v>
       </c>
       <c r="M7" s="39" t="str">
         <v>#N/A</v>
@@ -9376,10 +9540,10 @@
         <v>1</v>
       </c>
       <c r="O7" s="39">
-        <v>4.502117585177965E-2</v>
+        <v>4.5006928221515731E-2</v>
       </c>
       <c r="P7" s="39">
-        <v>9.9578001934688687E-4</v>
+        <v>9.9548657490292763E-4</v>
       </c>
       <c r="Q7" s="39">
         <v>0</v>
@@ -9399,22 +9563,22 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="B8" s="35">
-        <v>46857.793497313723</v>
+        <v>47112.214357766999</v>
       </c>
       <c r="C8" s="35">
         <v>1000000</v>
       </c>
       <c r="D8" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="E8" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="F8" s="36">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G8" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9423,16 +9587,16 @@
         <v>2</v>
       </c>
       <c r="I8" s="41">
-        <v>43962</v>
+        <v>44293</v>
       </c>
       <c r="J8" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K8" s="38">
-        <v>1.0138888888888888</v>
+        <v>1.0194444444444444</v>
       </c>
       <c r="L8" s="39">
-        <v>4.6215905915158749E-2</v>
+        <v>4.6213616263749646E-2</v>
       </c>
       <c r="M8" s="39" t="str">
         <v>#N/A</v>
@@ -9441,10 +9605,10 @@
         <v>1</v>
       </c>
       <c r="O8" s="39">
-        <v>4.5006928165107256E-2</v>
+        <v>4.5008034218931466E-2</v>
       </c>
       <c r="P8" s="39">
-        <v>1.2089777500514931E-3</v>
+        <v>1.2055820448181806E-3</v>
       </c>
       <c r="Q8" s="39">
         <v>0</v>
@@ -9464,19 +9628,19 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="B9" s="35">
-        <v>47078.945134035079</v>
+        <v>47090.565819230549</v>
       </c>
       <c r="C9" s="35">
         <v>1000000</v>
       </c>
       <c r="D9" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="E9" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="F9" s="36">
         <v>365</v>
@@ -9488,7 +9652,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="41">
-        <v>44327</v>
+        <v>44658</v>
       </c>
       <c r="J9" s="36" t="str">
         <v>Actual/360</v>
@@ -9497,7 +9661,7 @@
         <v>1.0138888888888888</v>
       </c>
       <c r="L9" s="39">
-        <v>4.643402807740446E-2</v>
+        <v>4.6445489575131504E-2</v>
       </c>
       <c r="M9" s="39" t="str">
         <v>#N/A</v>
@@ -9506,10 +9670,10 @@
         <v>1</v>
       </c>
       <c r="O9" s="39">
-        <v>4.500803415998271E-2</v>
+        <v>4.5019527592106562E-2</v>
       </c>
       <c r="P9" s="39">
-        <v>1.4259939174217501E-3</v>
+        <v>1.4259619830249426E-3</v>
       </c>
       <c r="Q9" s="39">
         <v>0</v>
@@ -9529,22 +9693,22 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="B10" s="35">
-        <v>47572.145779551589</v>
+        <v>47188.95522306973</v>
       </c>
       <c r="C10" s="35">
         <v>1000000</v>
       </c>
       <c r="D10" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="E10" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="F10" s="36">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G10" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9553,16 +9717,16 @@
         <v>2</v>
       </c>
       <c r="I10" s="41">
-        <v>44692</v>
+        <v>45021</v>
       </c>
       <c r="J10" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K10" s="38">
-        <v>1.0194444444444444</v>
+        <v>1.0111111111111111</v>
       </c>
       <c r="L10" s="39">
-        <v>4.6664775151603742E-2</v>
+        <v>4.6670395275563471E-2</v>
       </c>
       <c r="M10" s="39" t="str">
         <v>#N/A</v>
@@ -9571,10 +9735,10 @@
         <v>1</v>
       </c>
       <c r="O10" s="39">
-        <v>4.5019441051630464E-2</v>
+        <v>4.5021127210402197E-2</v>
       </c>
       <c r="P10" s="39">
-        <v>1.645334099973278E-3</v>
+        <v>1.6492680651612746E-3</v>
       </c>
       <c r="Q10" s="39">
         <v>0</v>
@@ -9594,22 +9758,22 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="B11" s="35">
-        <v>47421.574501604286</v>
+        <v>47531.46930844945</v>
       </c>
       <c r="C11" s="35">
         <v>1000000</v>
       </c>
       <c r="D11" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="E11" s="41">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="F11" s="36">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G11" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9618,16 +9782,16 @@
         <v>2</v>
       </c>
       <c r="I11" s="41">
-        <v>45057</v>
+        <v>45387</v>
       </c>
       <c r="J11" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K11" s="38">
-        <v>1.0111111111111111</v>
+        <v>1.0138888888888888</v>
       </c>
       <c r="L11" s="39">
-        <v>4.6900458298289954E-2</v>
+        <v>4.6880353290525492E-2</v>
       </c>
       <c r="M11" s="39" t="str">
         <v>#N/A</v>
@@ -9636,10 +9800,10 @@
         <v>1</v>
       </c>
       <c r="O11" s="39">
-        <v>4.5021175851779609E-2</v>
+        <v>4.5007071093443957E-2</v>
       </c>
       <c r="P11" s="39">
-        <v>1.8792824465103455E-3</v>
+        <v>1.8732821970815355E-3</v>
       </c>
       <c r="Q11" s="39">
         <v>0</v>

</xml_diff>

<commit_message>
merge with latest version
</commit_message>
<xml_diff>
--- a/QuantLibXL/StandaloneExamples/Analytics/InterestRateDerivatives.xlsx
+++ b/QuantLibXL/StandaloneExamples/Analytics/InterestRateDerivatives.xlsx
@@ -42,6 +42,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -54,6 +55,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -66,6 +68,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -78,6 +81,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>number of days to advance from EvaluationDate (usually zero or two): it fixes the date at which the discount factor = 1.0. If omitted, default = 0 is used.</t>
         </r>
@@ -90,6 +94,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>reference date</t>
         </r>
@@ -102,6 +107,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>cap/floor constant volatility Quote</t>
         </r>
@@ -114,6 +120,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>holiday calendar (e.g. TARGET) to advance from global EvaluationDate</t>
         </r>
@@ -126,6 +133,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>vol quotes</t>
         </r>
@@ -138,6 +146,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>holiday calendar (e.g. TARGET) used for calculating the exercise dates from the expiries</t>
         </r>
@@ -150,6 +159,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>the curve level</t>
         </r>
@@ -162,6 +172,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>DayCounter ID</t>
         </r>
@@ -174,6 +185,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>DayCounter ID</t>
         </r>
@@ -186,6 +198,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>DayCounter ID</t>
         </r>
@@ -198,6 +211,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -210,6 +224,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -222,6 +237,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Interest rate coumpounding rule (Simple:1+rt, Compounded:(1+r)^t, Continuous:e^{rt})</t>
         </r>
@@ -234,6 +250,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -246,6 +263,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -258,6 +276,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>frequency (e.g. Annual, Semiannual, Every4Month, Quarterly, Bimonthly, Monthly). If omitted, default = Annual is used.</t>
         </r>
@@ -270,6 +289,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -282,6 +302,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -304,6 +325,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -316,6 +338,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>effective date</t>
         </r>
@@ -328,6 +351,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>termination date</t>
         </r>
@@ -340,6 +364,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>tenor (e.g. 2D for two days , 3W for three weeks, 6M for six months, 1Y for one year)</t>
         </r>
@@ -352,6 +377,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>holiday calendar (e.g. TARGET)</t>
         </r>
@@ -364,6 +390,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>accrual dates business day convention</t>
         </r>
@@ -376,6 +403,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>termination date business day convention</t>
         </r>
@@ -388,6 +416,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Date generation rule (Backward, Forward, ThirdWednesday, Zero)</t>
         </r>
@@ -400,6 +429,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>end of month convention. FALSE by default.</t>
         </r>
@@ -412,6 +442,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>stub date, if there is an irregular starting period. NA by default.</t>
         </r>
@@ -424,6 +455,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>stub date, if there an irregular final period. NA by default.</t>
         </r>
@@ -436,6 +468,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -448,6 +481,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -460,6 +494,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -472,6 +507,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>effective date</t>
         </r>
@@ -484,6 +520,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>termination date</t>
         </r>
@@ -496,6 +533,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>tenor (e.g. 2D for two days , 3W for three weeks, 6M for six months, 1Y for one year)</t>
         </r>
@@ -508,6 +546,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>holiday calendar (e.g. TARGET)</t>
         </r>
@@ -520,6 +559,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>accrual dates business day convention</t>
         </r>
@@ -532,6 +572,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>termination date business day convention</t>
         </r>
@@ -544,6 +585,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Date generation rule (Backward, Forward, ThirdWednesday, Zero)</t>
         </r>
@@ -556,6 +598,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>end of month convention. FALSE by default.</t>
         </r>
@@ -568,6 +611,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>stub date, if there is an irregular starting period. NA by default.</t>
         </r>
@@ -580,6 +624,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>stub date, if there an irregular final period. NA by default.</t>
         </r>
@@ -592,6 +637,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -604,6 +650,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -626,6 +673,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -638,6 +686,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>discounting yield term structure object ID</t>
         </r>
@@ -650,6 +699,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -662,6 +712,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -674,6 +725,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -686,6 +738,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>discounting yield term structure object ID</t>
         </r>
@@ -698,6 +751,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>OptionletVolatilityStructure object ID</t>
         </r>
@@ -710,6 +764,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -722,6 +777,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -734,6 +790,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -746,6 +803,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>discounting yield term structure object ID</t>
         </r>
@@ -758,6 +816,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>SwaptionVolatilityStructure object ID</t>
         </r>
@@ -770,6 +829,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -782,6 +842,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -804,6 +865,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -816,6 +878,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -828,6 +891,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>index tenor (e.g. 3W for three weeks, 6M for six months, 1Y for one year)</t>
         </r>
@@ -840,6 +904,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>PAYER to pay the fixed rate, RECEIVER to receive it</t>
         </r>
@@ -852,6 +917,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>forecasting yield term structure</t>
         </r>
@@ -864,6 +930,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Notional Amount</t>
         </r>
@@ -876,6 +943,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -888,6 +956,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>fixed leg schedule object ID</t>
         </r>
@@ -900,6 +969,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -912,6 +982,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>the fixed rate</t>
         </r>
@@ -924,6 +995,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>fixed leg day counter (e.g. Actual/360)</t>
         </r>
@@ -936,6 +1008,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating leg schedule object ID</t>
         </r>
@@ -948,6 +1021,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating leg IborIndex object ID</t>
         </r>
@@ -960,6 +1034,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -972,6 +1047,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Index Spread</t>
         </r>
@@ -984,6 +1060,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>payment business day convention. If omitted, default = Following.</t>
         </r>
@@ -996,6 +1073,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating day counter (e.g. Actual/360)</t>
         </r>
@@ -1008,6 +1086,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Nominal amount vector. If omitted, default = 1000000</t>
         </r>
@@ -1020,6 +1099,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1032,6 +1112,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Schedule object ID</t>
         </r>
@@ -1044,6 +1125,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1056,6 +1138,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>fixing days (e.g. 2). If omitted, default = index natural fixing days</t>
         </r>
@@ -1068,6 +1151,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the fixing is in arrears. If omitted, default = FALSE</t>
         </r>
@@ -1080,6 +1164,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Payment DayCounter ID</t>
         </r>
@@ -1092,6 +1177,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floor strikes. If omitted, default = no floor</t>
         </r>
@@ -1104,6 +1190,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1116,6 +1203,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate gearings. If omitted, default = 1.0</t>
         </r>
@@ -1128,6 +1216,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>leg object IDs</t>
         </r>
@@ -1140,6 +1229,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate index</t>
         </r>
@@ -1152,6 +1242,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE for payed leg</t>
         </r>
@@ -1164,6 +1255,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate spreads. If omitted, default = 0%</t>
         </r>
@@ -1176,6 +1268,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1188,6 +1281,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>cap strikes. If omitted, default = no cap</t>
         </r>
@@ -1200,6 +1294,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1212,6 +1307,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1224,6 +1320,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1236,6 +1333,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1248,6 +1346,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>payment business day convention. If omitted, default = Following.</t>
         </r>
@@ -1260,6 +1359,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Nominal amount vector. If omitted, default = 1000000</t>
         </r>
@@ -1272,6 +1372,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Schedule object ID</t>
         </r>
@@ -1284,6 +1385,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>coupon fixed rates</t>
         </r>
@@ -1296,6 +1398,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Payment DayCounter ID</t>
         </r>
@@ -1308,6 +1411,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1320,6 +1424,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1342,6 +1447,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1354,6 +1460,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>option type (cap or floor)</t>
         </r>
@@ -1366,6 +1473,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>coupon vector</t>
         </r>
@@ -1378,6 +1486,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>strikes</t>
         </r>
@@ -1390,6 +1499,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1402,6 +1512,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1414,6 +1525,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1426,6 +1538,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>option type (cap or floor)</t>
         </r>
@@ -1438,6 +1551,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>coupon vector</t>
         </r>
@@ -1450,6 +1564,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>strikes</t>
         </r>
@@ -1462,6 +1577,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1474,6 +1590,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1496,6 +1613,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1508,6 +1626,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>expiry date</t>
         </r>
@@ -1520,6 +1639,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1532,6 +1652,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1544,6 +1665,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1556,6 +1678,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>underlying (vanilla) swap object ID</t>
         </r>
@@ -1568,6 +1691,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Exercise object ID</t>
         </r>
@@ -1580,6 +1704,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>settlement type (PhysicalSettlement, CashSettlement)</t>
         </r>
@@ -1592,6 +1717,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1604,6 +1730,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1626,6 +1753,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1638,6 +1766,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1650,6 +1779,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>index tenor (e.g. 1Y for one year)</t>
         </r>
@@ -1662,6 +1792,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>leg object IDs</t>
         </r>
@@ -1674,6 +1805,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>forecasting yield term structure</t>
         </r>
@@ -1686,6 +1818,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE for payed leg</t>
         </r>
@@ -1698,6 +1831,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1710,6 +1844,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1722,6 +1857,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1734,6 +1870,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1746,6 +1883,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1758,6 +1896,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Swaption Volatility Structure object ID</t>
         </r>
@@ -1770,6 +1909,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Cms Coupon Pricer Type (e.g ConundrumByBlack, ConundrumByNumericalIntegration, ClassicalAnaliticalFormula)</t>
         </r>
@@ -1782,6 +1922,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>model of the yield curve (e.g Standard, ExactYield, ParallelShifts, NonParallelShifts)</t>
         </r>
@@ -1794,6 +1935,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>mean reversion quote.</t>
         </r>
@@ -1806,6 +1948,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1818,6 +1961,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -1830,6 +1974,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>id of the object to be created. If missing a unique id will be automatically assigned.</t>
         </r>
@@ -1842,6 +1987,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>payment business day convention. If omitted, default = Following.</t>
         </r>
@@ -1854,6 +2000,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Nominal amount vector. If omitted, default = 1000000</t>
         </r>
@@ -1866,6 +2013,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Schedule object ID</t>
         </r>
@@ -1878,6 +2026,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>fixing days (e.g. 2). If omitted, default = index natural fixing days</t>
         </r>
@@ -1890,6 +2039,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the fixing is in arrears. If omitted, default = FALSE</t>
         </r>
@@ -1902,6 +2052,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Payment DayCounter ID</t>
         </r>
@@ -1914,6 +2065,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floor strikes. If omitted, default = no floor</t>
         </r>
@@ -1926,6 +2078,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate gearings. If omitted, default = 1.0</t>
         </r>
@@ -1938,6 +2091,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>underlying SwapIndex object ID</t>
         </r>
@@ -1950,6 +2104,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>floating rate spreads. If omitted, default = 0%</t>
         </r>
@@ -1962,6 +2117,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>cap strikes. If omitted, default = no cap</t>
         </r>
@@ -1974,6 +2130,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>TRUE if the object must be permanent (i.e. resistant to garbage collection). Default is FALSE.</t>
         </r>
@@ -1986,6 +2143,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Dependancy tracking trigger</t>
         </r>
@@ -2300,10 +2458,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.0000%"/>
-    <numFmt numFmtId="173" formatCode="ddd\,\ d\-mmm\-yyyy"/>
-    <numFmt numFmtId="176" formatCode="0.0000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="ddd\,\ d\-mmm\-yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -2313,11 +2471,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2481,10 +2641,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2503,7 +2663,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2515,9 +2675,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2550,17 +2710,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2572,19 +2732,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2891,7 +3057,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2912,21 +3078,21 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlFlatForward(B3,B4,B5,B6,B7,B8,B9,B10,B11)</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="11" t="str">
         <f>_xll.qlConstantSwaptionVolatility(E3,0,"TARGET","f",E5,E6,E7,E8)</f>
-        <v>obj_00050#0001</v>
+        <v>obj_00004#0016</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>96</v>
       </c>
       <c r="H1" s="11" t="str">
         <f>_xll.qlConstantOptionletVolatility(H3,0,H5,"f",H4,H6,H7,H8)</f>
-        <v>obj_0004d#0001</v>
+        <v>obj_00007#0010</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -2976,7 +3142,7 @@
       </c>
       <c r="E4" s="15">
         <f>_xll.qlSettingsEvaluationDate()</f>
-        <v>41768</v>
+        <v>42097</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>15</v>
@@ -2989,7 +3155,7 @@
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="43" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -3001,7 +3167,7 @@
       <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="43" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3039,7 +3205,7 @@
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -3055,7 +3221,7 @@
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="43" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3194,22 +3360,22 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="34">
-        <v>41956</v>
+        <v>42286</v>
       </c>
       <c r="B2" s="35">
-        <v>22428.645264951807</v>
+        <v>22305.401021215144</v>
       </c>
       <c r="C2" s="35">
         <v>1000000</v>
       </c>
       <c r="D2" s="41">
-        <v>41772</v>
+        <v>42103</v>
       </c>
       <c r="E2" s="41">
-        <v>41956</v>
+        <v>42286</v>
       </c>
       <c r="F2" s="36">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G2" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3218,16 +3384,16 @@
         <v>2</v>
       </c>
       <c r="I2" s="41">
-        <v>41768</v>
+        <v>42101</v>
       </c>
       <c r="J2" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K2" s="38">
-        <v>0.51111111111111107</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L2" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="M2" s="39" t="str">
         <v>#N/A</v>
@@ -3236,7 +3402,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="P2" s="39">
         <v>0</v>
@@ -3278,22 +3444,22 @@
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="34">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="B3" s="35">
-        <v>22058.957099786003</v>
+        <v>22551.90436642418</v>
       </c>
       <c r="C3" s="35">
         <v>1000000</v>
       </c>
       <c r="D3" s="41">
-        <v>41956</v>
+        <v>42286</v>
       </c>
       <c r="E3" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="F3" s="36">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G3" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3302,16 +3468,16 @@
         <v>2</v>
       </c>
       <c r="I3" s="41">
-        <v>41954</v>
+        <v>42284</v>
       </c>
       <c r="J3" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K3" s="38">
-        <v>0.50277777777777777</v>
+        <v>0.51388888888888884</v>
       </c>
       <c r="L3" s="39">
-        <v>4.3874168817253929E-2</v>
+        <v>4.3884786875203814E-2</v>
       </c>
       <c r="M3" s="39" t="str">
         <v>#N/A</v>
@@ -3320,7 +3486,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="39">
-        <v>4.3874168817253929E-2</v>
+        <v>4.3884786875203814E-2</v>
       </c>
       <c r="P3" s="39">
         <v>0</v>
@@ -3362,22 +3528,22 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="34">
-        <v>42321</v>
+        <v>42653</v>
       </c>
       <c r="B4" s="35">
-        <v>22428.645264951811</v>
+        <v>22182.171633423619</v>
       </c>
       <c r="C4" s="35">
         <v>1000000</v>
       </c>
       <c r="D4" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="E4" s="41">
-        <v>42321</v>
+        <v>42653</v>
       </c>
       <c r="F4" s="36">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G4" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3386,16 +3552,16 @@
         <v>2</v>
       </c>
       <c r="I4" s="41">
-        <v>42135</v>
+        <v>42467</v>
       </c>
       <c r="J4" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K4" s="38">
-        <v>0.51111111111111107</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="L4" s="39">
-        <v>4.388213204012311E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="M4" s="39" t="str">
         <v>#N/A</v>
@@ -3404,10 +3570,10 @@
         <v>1</v>
       </c>
       <c r="O4" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="P4" s="39">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="39">
         <v>0</v>
@@ -3446,7 +3612,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="34">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="B5" s="35">
         <v>22182.171633423615</v>
@@ -3455,10 +3621,10 @@
         <v>1000000</v>
       </c>
       <c r="D5" s="41">
-        <v>42321</v>
+        <v>42653</v>
       </c>
       <c r="E5" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="F5" s="36">
         <v>182</v>
@@ -3470,7 +3636,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="41">
-        <v>42319</v>
+        <v>42649</v>
       </c>
       <c r="J5" s="36" t="str">
         <v>Actual/360</v>
@@ -3530,22 +3696,22 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="34">
-        <v>42688</v>
+        <v>43017</v>
       </c>
       <c r="B6" s="35">
-        <v>22551.904366423958</v>
+        <v>22182.171633423615</v>
       </c>
       <c r="C6" s="35">
         <v>1000000</v>
       </c>
       <c r="D6" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="E6" s="41">
-        <v>42688</v>
+        <v>43017</v>
       </c>
       <c r="F6" s="36">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G6" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3554,16 +3720,16 @@
         <v>2</v>
       </c>
       <c r="I6" s="41">
-        <v>42501</v>
+        <v>42831</v>
       </c>
       <c r="J6" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K6" s="38">
-        <v>0.51388888888888884</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="L6" s="39">
-        <v>4.3884786875203384E-2</v>
+        <v>4.3876823011167597E-2</v>
       </c>
       <c r="M6" s="39" t="str">
         <v>#N/A</v>
@@ -3572,10 +3738,10 @@
         <v>1</v>
       </c>
       <c r="O6" s="39">
-        <v>4.3884786875203384E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="P6" s="39">
-        <v>0</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="Q6" s="39">
         <v>0</v>
@@ -3614,7 +3780,7 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="34">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="B7" s="35">
         <v>22182.171633423619</v>
@@ -3623,10 +3789,10 @@
         <v>1000000</v>
       </c>
       <c r="D7" s="41">
-        <v>42688</v>
+        <v>43017</v>
       </c>
       <c r="E7" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="F7" s="36">
         <v>182</v>
@@ -3638,7 +3804,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="41">
-        <v>42684</v>
+        <v>43013</v>
       </c>
       <c r="J7" s="36" t="str">
         <v>Actual/360</v>
@@ -3698,22 +3864,22 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
-        <v>43052</v>
+        <v>43382</v>
       </c>
       <c r="B8" s="35">
-        <v>22182.171633423619</v>
+        <v>22305.401021215366</v>
       </c>
       <c r="C8" s="35">
         <v>1000000</v>
       </c>
       <c r="D8" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="E8" s="41">
-        <v>43052</v>
+        <v>43382</v>
       </c>
       <c r="F8" s="36">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G8" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3722,16 +3888,16 @@
         <v>2</v>
       </c>
       <c r="I8" s="41">
-        <v>42866</v>
+        <v>43195</v>
       </c>
       <c r="J8" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K8" s="38">
-        <v>0.50555555555555554</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L8" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="M8" s="39" t="str">
         <v>#N/A</v>
@@ -3740,7 +3906,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="P8" s="39">
         <v>0</v>
@@ -3782,19 +3948,19 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="B9" s="35">
-        <v>22182.171633423397</v>
+        <v>22182.171633423615</v>
       </c>
       <c r="C9" s="35">
         <v>1000000</v>
       </c>
       <c r="D9" s="41">
-        <v>43052</v>
+        <v>43382</v>
       </c>
       <c r="E9" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="F9" s="36">
         <v>182</v>
@@ -3806,7 +3972,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="41">
-        <v>43048</v>
+        <v>43378</v>
       </c>
       <c r="J9" s="36" t="str">
         <v>Actual/360</v>
@@ -3815,7 +3981,7 @@
         <v>0.50555555555555554</v>
       </c>
       <c r="L9" s="39">
-        <v>4.387682301116716E-2</v>
+        <v>4.3876823011167597E-2</v>
       </c>
       <c r="M9" s="39" t="str">
         <v>#N/A</v>
@@ -3824,10 +3990,10 @@
         <v>1</v>
       </c>
       <c r="O9" s="39">
-        <v>4.387682301116716E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="P9" s="39">
-        <v>0</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="Q9" s="39">
         <v>0</v>
@@ -3866,19 +4032,19 @@
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
-        <v>43417</v>
+        <v>43747</v>
       </c>
       <c r="B10" s="35">
-        <v>22305.40102121537</v>
+        <v>22305.401021215144</v>
       </c>
       <c r="C10" s="35">
         <v>1000000</v>
       </c>
       <c r="D10" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="E10" s="41">
-        <v>43417</v>
+        <v>43747</v>
       </c>
       <c r="F10" s="36">
         <v>183</v>
@@ -3890,7 +4056,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="41">
-        <v>43230</v>
+        <v>43560</v>
       </c>
       <c r="J10" s="36" t="str">
         <v>Actual/360</v>
@@ -3899,7 +4065,7 @@
         <v>0.5083333333333333</v>
       </c>
       <c r="L10" s="39">
-        <v>4.3879477418784334E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="M10" s="39" t="str">
         <v>#N/A</v>
@@ -3908,10 +4074,10 @@
         <v>1</v>
       </c>
       <c r="O10" s="39">
-        <v>4.3879477418784327E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="P10" s="39">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="39">
         <v>0</v>
@@ -3950,22 +4116,22 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="B11" s="35">
-        <v>22058.957099786003</v>
+        <v>22305.401021215144</v>
       </c>
       <c r="C11" s="35">
         <v>1000000</v>
       </c>
       <c r="D11" s="41">
-        <v>43417</v>
+        <v>43747</v>
       </c>
       <c r="E11" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="F11" s="36">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G11" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -3974,16 +4140,16 @@
         <v>2</v>
       </c>
       <c r="I11" s="41">
-        <v>43413</v>
+        <v>43745</v>
       </c>
       <c r="J11" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K11" s="38">
-        <v>0.50277777777777777</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L11" s="39">
-        <v>4.3874168817253929E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="M11" s="39" t="str">
         <v>#N/A</v>
@@ -3992,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="39">
-        <v>4.3874168817253929E-2</v>
+        <v>4.387947741878389E-2</v>
       </c>
       <c r="P11" s="39">
         <v>0</v>
@@ -4034,22 +4200,22 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="34">
-        <v>43782</v>
+        <v>44113</v>
       </c>
       <c r="B12" s="35">
-        <v>22428.645264951807</v>
+        <v>22305.40102121537</v>
       </c>
       <c r="C12" s="35">
         <v>1000000</v>
       </c>
       <c r="D12" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="E12" s="41">
-        <v>43782</v>
+        <v>44113</v>
       </c>
       <c r="F12" s="36">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G12" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4058,16 +4224,16 @@
         <v>2</v>
       </c>
       <c r="I12" s="41">
-        <v>43594</v>
+        <v>43928</v>
       </c>
       <c r="J12" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K12" s="38">
-        <v>0.51111111111111107</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L12" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3879477418784334E-2</v>
       </c>
       <c r="M12" s="39" t="str">
         <v>#N/A</v>
@@ -4076,10 +4242,10 @@
         <v>1</v>
       </c>
       <c r="O12" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="P12" s="39">
-        <v>0</v>
+        <v>6.9388939039072284E-18</v>
       </c>
       <c r="Q12" s="39">
         <v>0</v>
@@ -4118,7 +4284,7 @@
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="34">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="B13" s="35">
         <v>22182.171633423615</v>
@@ -4127,10 +4293,10 @@
         <v>1000000</v>
       </c>
       <c r="D13" s="41">
-        <v>43782</v>
+        <v>44113</v>
       </c>
       <c r="E13" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="F13" s="36">
         <v>182</v>
@@ -4142,7 +4308,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="41">
-        <v>43780</v>
+        <v>44111</v>
       </c>
       <c r="J13" s="36" t="str">
         <v>Actual/360</v>
@@ -4202,22 +4368,22 @@
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="34">
-        <v>44148</v>
+        <v>44480</v>
       </c>
       <c r="B14" s="35">
-        <v>22428.645264951807</v>
+        <v>22551.90436642418</v>
       </c>
       <c r="C14" s="35">
         <v>1000000</v>
       </c>
       <c r="D14" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="E14" s="41">
-        <v>44148</v>
+        <v>44480</v>
       </c>
       <c r="F14" s="36">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G14" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4226,16 +4392,16 @@
         <v>2</v>
       </c>
       <c r="I14" s="41">
-        <v>43962</v>
+        <v>44293</v>
       </c>
       <c r="J14" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K14" s="38">
-        <v>0.51111111111111107</v>
+        <v>0.51388888888888884</v>
       </c>
       <c r="L14" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3884786875203814E-2</v>
       </c>
       <c r="M14" s="39" t="str">
         <v>#N/A</v>
@@ -4244,7 +4410,7 @@
         <v>1</v>
       </c>
       <c r="O14" s="39">
-        <v>4.3882132040123104E-2</v>
+        <v>4.3884786875203814E-2</v>
       </c>
       <c r="P14" s="39">
         <v>0</v>
@@ -4286,22 +4452,22 @@
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="34">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="B15" s="35">
-        <v>22058.957099786221</v>
+        <v>22182.171633423619</v>
       </c>
       <c r="C15" s="35">
         <v>1000000</v>
       </c>
       <c r="D15" s="41">
-        <v>44148</v>
+        <v>44480</v>
       </c>
       <c r="E15" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="F15" s="36">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G15" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4310,16 +4476,16 @@
         <v>2</v>
       </c>
       <c r="I15" s="41">
-        <v>44146</v>
+        <v>44476</v>
       </c>
       <c r="J15" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K15" s="38">
-        <v>0.50277777777777777</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="L15" s="39">
-        <v>4.3874168817254366E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="M15" s="39" t="str">
         <v>#N/A</v>
@@ -4328,10 +4494,10 @@
         <v>1</v>
       </c>
       <c r="O15" s="39">
-        <v>4.3874168817254373E-2</v>
+        <v>4.3876823011167604E-2</v>
       </c>
       <c r="P15" s="39">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="39">
         <v>0</v>
@@ -4370,22 +4536,22 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="34">
-        <v>44515</v>
+        <v>44844</v>
       </c>
       <c r="B16" s="35">
-        <v>22675.178327423273</v>
+        <v>22182.171633423397</v>
       </c>
       <c r="C16" s="35">
         <v>1000000</v>
       </c>
       <c r="D16" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="E16" s="41">
-        <v>44515</v>
+        <v>44844</v>
       </c>
       <c r="F16" s="36">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G16" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4394,16 +4560,16 @@
         <v>2</v>
       </c>
       <c r="I16" s="41">
-        <v>44327</v>
+        <v>44658</v>
       </c>
       <c r="J16" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K16" s="38">
-        <v>0.51666666666666672</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="L16" s="39">
-        <v>4.3887441924045041E-2</v>
+        <v>4.387682301116716E-2</v>
       </c>
       <c r="M16" s="39" t="str">
         <v>#N/A</v>
@@ -4412,7 +4578,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="39">
-        <v>4.3887441924045041E-2</v>
+        <v>4.387682301116716E-2</v>
       </c>
       <c r="P16" s="39">
         <v>0</v>
@@ -4454,22 +4620,22 @@
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="34">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="B17" s="35">
-        <v>21812.572587811996</v>
+        <v>22305.401021215366</v>
       </c>
       <c r="C17" s="35">
         <v>1000000</v>
       </c>
       <c r="D17" s="41">
-        <v>44515</v>
+        <v>44844</v>
       </c>
       <c r="E17" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="F17" s="36">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G17" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4478,16 +4644,16 @@
         <v>2</v>
       </c>
       <c r="I17" s="41">
-        <v>44511</v>
+        <v>44840</v>
       </c>
       <c r="J17" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K17" s="38">
-        <v>0.49722222222222223</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L17" s="39">
-        <v>4.3868861070459876E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="M17" s="39" t="str">
         <v>#N/A</v>
@@ -4496,7 +4662,7 @@
         <v>1</v>
       </c>
       <c r="O17" s="39">
-        <v>4.3868861070459876E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="P17" s="39">
         <v>0</v>
@@ -4538,22 +4704,22 @@
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="34">
-        <v>44879</v>
+        <v>45208</v>
       </c>
       <c r="B18" s="35">
-        <v>22551.904366423954</v>
+        <v>22058.957099786221</v>
       </c>
       <c r="C18" s="35">
         <v>1000000</v>
       </c>
       <c r="D18" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="E18" s="41">
-        <v>44879</v>
+        <v>45208</v>
       </c>
       <c r="F18" s="36">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G18" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4562,16 +4728,16 @@
         <v>2</v>
       </c>
       <c r="I18" s="41">
-        <v>44692</v>
+        <v>45021</v>
       </c>
       <c r="J18" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K18" s="38">
-        <v>0.51388888888888884</v>
+        <v>0.50277777777777777</v>
       </c>
       <c r="L18" s="39">
-        <v>4.3884786875203377E-2</v>
+        <v>4.3874168817254366E-2</v>
       </c>
       <c r="M18" s="39" t="str">
         <v>#N/A</v>
@@ -4580,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="O18" s="39">
-        <v>4.3884786875203384E-2</v>
+        <v>4.3874168817254373E-2</v>
       </c>
       <c r="P18" s="39">
         <v>-6.9388939039072284E-18</v>
@@ -4622,22 +4788,22 @@
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="34">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="B19" s="35">
-        <v>22182.171633423619</v>
+        <v>22305.401021215366</v>
       </c>
       <c r="C19" s="35">
         <v>1000000</v>
       </c>
       <c r="D19" s="41">
-        <v>44879</v>
+        <v>45208</v>
       </c>
       <c r="E19" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="F19" s="36">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G19" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4646,16 +4812,16 @@
         <v>2</v>
       </c>
       <c r="I19" s="41">
-        <v>44875</v>
+        <v>45204</v>
       </c>
       <c r="J19" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K19" s="38">
-        <v>0.50555555555555554</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L19" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="M19" s="39" t="str">
         <v>#N/A</v>
@@ -4664,7 +4830,7 @@
         <v>1</v>
       </c>
       <c r="O19" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418784327E-2</v>
       </c>
       <c r="P19" s="39">
         <v>0</v>
@@ -4706,22 +4872,22 @@
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="34">
-        <v>45243</v>
+        <v>45574</v>
       </c>
       <c r="B20" s="35">
-        <v>22182.171633423615</v>
+        <v>22305.401021214922</v>
       </c>
       <c r="C20" s="35">
         <v>1000000</v>
       </c>
       <c r="D20" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="E20" s="41">
-        <v>45243</v>
+        <v>45574</v>
       </c>
       <c r="F20" s="36">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G20" s="37" t="str">
         <v>Euribor6M Actual/360</v>
@@ -4730,16 +4896,16 @@
         <v>2</v>
       </c>
       <c r="I20" s="41">
-        <v>45057</v>
+        <v>45387</v>
       </c>
       <c r="J20" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K20" s="38">
-        <v>0.50555555555555554</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="L20" s="39">
-        <v>4.3876823011167597E-2</v>
+        <v>4.3879477418783452E-2</v>
       </c>
       <c r="M20" s="39" t="str">
         <v>#N/A</v>
@@ -4748,10 +4914,10 @@
         <v>1</v>
       </c>
       <c r="O20" s="39">
-        <v>4.3876823011167604E-2</v>
+        <v>4.3879477418783452E-2</v>
       </c>
       <c r="P20" s="39">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="39">
         <v>0</v>
@@ -4790,19 +4956,19 @@
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="34">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="B21" s="35">
-        <v>22182.171633423401</v>
+        <v>22182.171633423841</v>
       </c>
       <c r="C21" s="35">
         <v>1000000</v>
       </c>
       <c r="D21" s="41">
-        <v>45243</v>
+        <v>45574</v>
       </c>
       <c r="E21" s="41">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="F21" s="36">
         <v>182</v>
@@ -4814,7 +4980,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="41">
-        <v>45239</v>
+        <v>45572</v>
       </c>
       <c r="J21" s="36" t="str">
         <v>Actual/360</v>
@@ -4823,7 +4989,7 @@
         <v>0.50555555555555554</v>
       </c>
       <c r="L21" s="39">
-        <v>4.3876823011167167E-2</v>
+        <v>4.3876823011168041E-2</v>
       </c>
       <c r="M21" s="39" t="str">
         <v>#N/A</v>
@@ -4832,10 +4998,10 @@
         <v>1</v>
       </c>
       <c r="O21" s="39">
-        <v>4.387682301116716E-2</v>
+        <v>4.3876823011168041E-2</v>
       </c>
       <c r="P21" s="39">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="39">
         <v>0</v>
@@ -5179,7 +5345,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5195,7 +5361,7 @@
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="44" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5204,8 +5370,8 @@
         <v>35</v>
       </c>
       <c r="B2" s="15">
-        <f>_xll.qlCalendarAdvance(Calendar,ReferenceDate,"2d")</f>
-        <v>41772</v>
+        <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdjust(Calendar,ReferenceDate,"f"),"2d")</f>
+        <v>42103</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5214,7 +5380,7 @@
       </c>
       <c r="B3" s="29">
         <f>_xll.qlCalendarAdvance(Calendar,B2,"10Y","Unadjusted")</f>
-        <v>45425</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -5224,7 +5390,7 @@
       </c>
       <c r="B5" s="11" t="str">
         <f>_xll.qlSchedule(B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19)</f>
-        <v>obj_00051#0001</v>
+        <v>obj_00009#0013</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5248,7 +5414,7 @@
       </c>
       <c r="B8" s="15">
         <f>EffectiveDate</f>
-        <v>41772</v>
+        <v>42103</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -5257,7 +5423,7 @@
       </c>
       <c r="B9" s="15">
         <f>TerminationDate</f>
-        <v>45425</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -5337,7 +5503,7 @@
       </c>
       <c r="B21" s="11" t="str">
         <f>_xll.qlSchedule(B23,B24,B25,B26,B27,B28,B29,B30,B31,B32,B33,B34,B35)</f>
-        <v>obj_00052#0001</v>
+        <v>obj_0000a#0013</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5361,7 +5527,7 @@
       </c>
       <c r="B24" s="15">
         <f>EffectiveDate</f>
-        <v>41772</v>
+        <v>42103</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -5370,7 +5536,7 @@
       </c>
       <c r="B25" s="15">
         <f>TerminationDate</f>
-        <v>45425</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -5465,7 +5631,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5480,7 +5646,7 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlDiscountingSwapEngine(B3,B4,B5,B6)</f>
-        <v>obj_00054#0001</v>
+        <v>obj_00001#0020</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5504,7 +5670,7 @@
       </c>
       <c r="B4" s="8" t="str">
         <f>TermStructures!$B$1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -5526,7 +5692,7 @@
       </c>
       <c r="B8" s="11" t="str">
         <f>_xll.qlBlackCapFloorEngine(B10,B11,B12,B13,B14)</f>
-        <v>obj_00057#0001</v>
+        <v>obj_00008#0021</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5550,7 +5716,7 @@
       </c>
       <c r="B11" s="8" t="str">
         <f>TermStructures!$B$1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5559,7 +5725,7 @@
       </c>
       <c r="B12" s="8" t="str">
         <f>TermStructures!$H$1</f>
-        <v>obj_0004d#0001</v>
+        <v>obj_00007#0010</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -5581,7 +5747,7 @@
       </c>
       <c r="B16" s="11" t="str">
         <f>_xll.qlBlackSwaptionEngine(B18,B19,B20,B21,B22)</f>
-        <v>obj_00055#0001</v>
+        <v>obj_00006#0021</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5605,7 +5771,7 @@
       </c>
       <c r="B19" s="8" t="str">
         <f>TermStructures!$B$1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -5614,7 +5780,7 @@
       </c>
       <c r="B20" s="8" t="str">
         <f>TermStructures!$E$1</f>
-        <v>obj_00050#0001</v>
+        <v>obj_00004#0016</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -5643,7 +5809,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5665,14 +5831,14 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlEuribor(B3,B4,B5,B6,B7)</f>
-        <v>obj_00058#0001</v>
+        <v>obj_00003#0024</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="11" t="str">
         <f>_xll.qlVanillaSwap(E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14)</f>
-        <v>obj_0005c#0001</v>
+        <v>obj_0000c#0028</v>
       </c>
       <c r="H1" t="s">
         <v>75</v>
@@ -5702,7 +5868,7 @@
       </c>
       <c r="I2" s="27">
         <f>_xll.qlInstrumentNPV(E1,I1)</f>
-        <v>-39387.492820908315</v>
+        <v>-39363.257108460588</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5719,7 +5885,7 @@
       </c>
       <c r="I3" s="28">
         <f>_xll.qlVanillaSwapFairRate($E$1,$I$1)</f>
-        <v>4.5019439201856769E-2</v>
+        <v>4.5021117962698143E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5741,7 +5907,7 @@
       </c>
       <c r="I4" s="28">
         <f>_xll.qlVanillaSwapFairSpread($E$1,$I$1)</f>
-        <v>4.8543530153119544E-3</v>
+        <v>4.8525326129049808E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5750,7 +5916,7 @@
       </c>
       <c r="B5" s="8" t="str">
         <f>TermStructures!B1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>23</v>
@@ -5770,7 +5936,7 @@
       </c>
       <c r="E6" s="8" t="str">
         <f>DateCalc!$B$5</f>
-        <v>obj_00051#0001</v>
+        <v>obj_00009#0013</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5801,14 +5967,14 @@
       </c>
       <c r="B9" s="11" t="str">
         <f>_xll.qlIborLeg(B11,B12,B13,B14,B15,B16,B17,B18,B19,B20,B21,B22,B23,B24)</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="8" t="str">
         <f>DateCalc!B21</f>
-        <v>obj_00052#0001</v>
+        <v>obj_0000a#0013</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5824,7 +5990,7 @@
       </c>
       <c r="E10" s="8" t="str">
         <f>B1</f>
-        <v>obj_00058#0001</v>
+        <v>obj_00003#0024</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5873,7 +6039,7 @@
       </c>
       <c r="B14" s="8" t="str">
         <f>DateCalc!B21</f>
-        <v>obj_00052#0001</v>
+        <v>obj_0000a#0013</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>11</v>
@@ -5896,7 +6062,7 @@
       </c>
       <c r="E16" s="11" t="str">
         <f>_xll.qlSwap(E18,E19:F19,E20:F20,E21,E22)</f>
-        <v>obj_00060#0001</v>
+        <v>obj_00010#0020</v>
       </c>
       <c r="H16" t="s">
         <v>75</v>
@@ -5925,7 +6091,7 @@
       </c>
       <c r="I17" s="27">
         <f>_xll.qlInstrumentNPV(E16,I16)</f>
-        <v>-39387.492820908315</v>
+        <v>-39363.257108460588</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5949,11 +6115,11 @@
       </c>
       <c r="E19" s="17" t="str">
         <f>B26</f>
-        <v>obj_0005b#0001</v>
+        <v>obj_0000b#0013</v>
       </c>
       <c r="F19" s="18" t="str">
         <f>B9</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -5962,7 +6128,7 @@
       </c>
       <c r="B20" s="8" t="str">
         <f>B1</f>
-        <v>obj_00058#0001</v>
+        <v>obj_00003#0024</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>18</v>
@@ -6013,7 +6179,7 @@
       </c>
       <c r="B26" s="11" t="str">
         <f>_xll.qlFixedRateLeg(B28,B29,B30,B31,B32,B33,B34,B35)</f>
-        <v>obj_0005b#0001</v>
+        <v>obj_0000b#0013</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6054,7 +6220,7 @@
       </c>
       <c r="B31" s="8" t="str">
         <f>DateCalc!$B$5</f>
-        <v>obj_00051#0001</v>
+        <v>obj_00009#0013</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -6087,7 +6253,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
       <formula1>"Payer,Receiver"</formula1>
     </dataValidation>
@@ -6128,7 +6294,7 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlCapFloor(B3,B4,B5,B6,B7,B8)</f>
-        <v>obj_0005f#0001</v>
+        <v>obj_00012#0020</v>
       </c>
       <c r="D1" t="s">
         <v>75</v>
@@ -6151,7 +6317,7 @@
       </c>
       <c r="E2" s="27">
         <f>_xll.qlInstrumentNPV(B1,E1)</f>
-        <v>26215.851935305589</v>
+        <v>26175.177192398387</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -6164,7 +6330,7 @@
       </c>
       <c r="E3" s="2">
         <f>_xll.qlCapFloorAtmRate(B1,TermStructures!$B$1)</f>
-        <v>4.3878643248097524E-2</v>
+        <v>4.3878614023525997E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -6188,7 +6354,7 @@
       </c>
       <c r="B5" s="8" t="str">
         <f>Swaps!B9</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -6218,7 +6384,7 @@
       </c>
       <c r="B10" s="11" t="str">
         <f>_xll.qlCapFloor(B12,B13,B14,B15,B16,B17)</f>
-        <v>obj_0005e#0001</v>
+        <v>obj_0000f#0020</v>
       </c>
       <c r="D10" t="s">
         <v>75</v>
@@ -6241,7 +6407,7 @@
       </c>
       <c r="E11" s="27">
         <f>_xll.qlInstrumentNPV(B10,E10)</f>
-        <v>57686.58193937147</v>
+        <v>57638.1045360512</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -6254,7 +6420,7 @@
       </c>
       <c r="E12" s="2">
         <f>_xll.qlCapFloorAtmRate(B10,TermStructures!$B$1)</f>
-        <v>4.3878643248097524E-2</v>
+        <v>4.3878614023525997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -6278,7 +6444,7 @@
       </c>
       <c r="B14" s="8" t="str">
         <f>Swaps!B9</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -6337,7 +6503,7 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlEuropeanExercise(B3,B4,B5,B6)</f>
-        <v>obj_0004e#0001</v>
+        <v>obj_00013#0005</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6382,7 +6548,7 @@
       </c>
       <c r="B8" s="11" t="str">
         <f>_xll.qlSwaption(B10,B11,B12,B13,B14,B15)</f>
-        <v>obj_0005d#0001</v>
+        <v>obj_00014#0018</v>
       </c>
       <c r="D8" t="s">
         <v>75</v>
@@ -6405,7 +6571,7 @@
       </c>
       <c r="E9" s="27">
         <f>_xll.qlInstrumentNPV(B8,E8)</f>
-        <v>8034.9988082185755</v>
+        <v>7964.1828023073604</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -6427,7 +6593,7 @@
       </c>
       <c r="B11" s="8" t="str">
         <f>Swaps!E1</f>
-        <v>obj_0005c#0001</v>
+        <v>obj_0000c#0028</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -6436,7 +6602,7 @@
       </c>
       <c r="B12" s="8" t="str">
         <f>B1</f>
-        <v>obj_0004e#0001</v>
+        <v>obj_00013#0005</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -6499,14 +6665,14 @@
       </c>
       <c r="B1" s="11" t="str">
         <f>_xll.qlEuriborSwapIsdaFixA(B3,B4,B5,B6,B7,B8)</f>
-        <v>obj_00056#0001</v>
+        <v>obj_00002#0020</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E1" s="11" t="str">
         <f>_xll.qlSwap(E3,E4:F4,E5:F5,E6,E7)</f>
-        <v>obj_00061#0001</v>
+        <v>obj_00011#0020</v>
       </c>
       <c r="H1" t="s">
         <v>75</v>
@@ -6536,7 +6702,7 @@
       </c>
       <c r="I2" s="27">
         <f>_xll.qlInstrumentNPV(E1,I1)</f>
-        <v>-11903.469893039088</v>
+        <v>-11879.445724761754</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6562,11 +6728,11 @@
       </c>
       <c r="E4" s="17" t="str">
         <f>B20</f>
-        <v>obj_0005a#0001</v>
+        <v>obj_0000e#0019</v>
       </c>
       <c r="F4" s="18" t="str">
         <f>Swaps!B9</f>
-        <v>obj_00059#0001</v>
+        <v>obj_0000d#0020</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6575,7 +6741,7 @@
       </c>
       <c r="B5" s="8" t="str">
         <f>TermStructures!B1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>18</v>
@@ -6593,7 +6759,7 @@
       </c>
       <c r="B6" s="8" t="str">
         <f>TermStructures!B1</f>
-        <v>obj_0004f#0001</v>
+        <v>obj_00000#0020</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>10</v>
@@ -6623,7 +6789,7 @@
       </c>
       <c r="B10" s="11" t="str">
         <f>_xll.qlCmsCouponPricer(B12,B13,B14,B15,B16,B17,B18)</f>
-        <v>obj_00053#0001</v>
+        <v>obj_00005#0010</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6647,7 +6813,7 @@
       </c>
       <c r="B13" s="8" t="str">
         <f>TermStructures!E1</f>
-        <v>obj_00050#0001</v>
+        <v>obj_00004#0016</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -6693,7 +6859,7 @@
       </c>
       <c r="B20" s="11" t="str">
         <f>_xll.qlCmsLeg(B22,B23,B24,B25,B26,B27,B28,B29,B30,B31,B32,B33,B34,B35)</f>
-        <v>obj_0005a#0001</v>
+        <v>obj_0000e#0019</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -6734,7 +6900,7 @@
       </c>
       <c r="B25" s="8" t="str">
         <f>DateCalc!B5</f>
-        <v>obj_00051#0001</v>
+        <v>obj_00009#0013</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -6775,7 +6941,7 @@
       </c>
       <c r="B31" s="8" t="str">
         <f>B1</f>
-        <v>obj_00056#0001</v>
+        <v>obj_00002#0020</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -6931,22 +7097,22 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="34">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="B2" s="35">
-        <v>50000.000000000044</v>
+        <v>50277.777777777868</v>
       </c>
       <c r="C2" s="35">
         <v>1000000</v>
       </c>
       <c r="D2" s="41">
-        <v>41772</v>
+        <v>42103</v>
       </c>
       <c r="E2" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="F2" s="36">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G2" s="37" t="str">
         <v>#N/A</v>
@@ -6961,7 +7127,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K2" s="38">
-        <v>1</v>
+        <v>1.0055555555555555</v>
       </c>
       <c r="L2" s="39">
         <v>0.05</v>
@@ -7015,22 +7181,22 @@
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="34">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="B3" s="35">
-        <v>50000.000000000044</v>
+        <v>49861.111111111131</v>
       </c>
       <c r="C3" s="35">
         <v>1000000</v>
       </c>
       <c r="D3" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="E3" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="F3" s="36">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G3" s="37" t="str">
         <v>#N/A</v>
@@ -7045,7 +7211,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K3" s="38">
-        <v>1</v>
+        <v>0.99722222222222223</v>
       </c>
       <c r="L3" s="39">
         <v>0.05</v>
@@ -7099,22 +7265,22 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="34">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="B4" s="35">
-        <v>50277.777777777868</v>
+        <v>49861.111111111131</v>
       </c>
       <c r="C4" s="35">
         <v>1000000</v>
       </c>
       <c r="D4" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="E4" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="F4" s="36">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G4" s="37" t="str">
         <v>#N/A</v>
@@ -7129,7 +7295,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K4" s="38">
-        <v>1.0055555555555555</v>
+        <v>0.99722222222222223</v>
       </c>
       <c r="L4" s="39">
         <v>0.05</v>
@@ -7183,22 +7349,22 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="34">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="B5" s="35">
-        <v>49861.111111111131</v>
+        <v>50000.000000000044</v>
       </c>
       <c r="C5" s="35">
         <v>1000000</v>
       </c>
       <c r="D5" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="E5" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="F5" s="36">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G5" s="37" t="str">
         <v>#N/A</v>
@@ -7213,7 +7379,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K5" s="38">
-        <v>0.99722222222222223</v>
+        <v>1</v>
       </c>
       <c r="L5" s="39">
         <v>0.05</v>
@@ -7267,22 +7433,22 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="34">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="B6" s="35">
-        <v>49861.111111111131</v>
+        <v>50000.000000000044</v>
       </c>
       <c r="C6" s="35">
         <v>1000000</v>
       </c>
       <c r="D6" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="E6" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="F6" s="36">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G6" s="37" t="str">
         <v>#N/A</v>
@@ -7297,7 +7463,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K6" s="38">
-        <v>0.99722222222222223</v>
+        <v>1</v>
       </c>
       <c r="L6" s="39">
         <v>0.05</v>
@@ -7351,7 +7517,7 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="34">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="B7" s="35">
         <v>50000.000000000044</v>
@@ -7360,10 +7526,10 @@
         <v>1000000</v>
       </c>
       <c r="D7" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="E7" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="F7" s="36">
         <v>360</v>
@@ -7435,22 +7601,22 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="B8" s="35">
-        <v>50000.000000000044</v>
+        <v>50277.777777777868</v>
       </c>
       <c r="C8" s="35">
         <v>1000000</v>
       </c>
       <c r="D8" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="E8" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="F8" s="36">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G8" s="37" t="str">
         <v>#N/A</v>
@@ -7465,7 +7631,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K8" s="38">
-        <v>1</v>
+        <v>1.0055555555555555</v>
       </c>
       <c r="L8" s="39">
         <v>0.05</v>
@@ -7519,7 +7685,7 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="B9" s="35">
         <v>50000.000000000044</v>
@@ -7528,10 +7694,10 @@
         <v>1000000</v>
       </c>
       <c r="D9" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="E9" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="F9" s="36">
         <v>360</v>
@@ -7603,22 +7769,22 @@
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="B10" s="35">
-        <v>50277.777777777868</v>
+        <v>49722.222222222226</v>
       </c>
       <c r="C10" s="35">
         <v>1000000</v>
       </c>
       <c r="D10" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="E10" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="F10" s="36">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G10" s="37" t="str">
         <v>#N/A</v>
@@ -7633,7 +7799,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K10" s="38">
-        <v>1.0055555555555555</v>
+        <v>0.99444444444444446</v>
       </c>
       <c r="L10" s="39">
         <v>0.05</v>
@@ -7687,22 +7853,22 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="B11" s="35">
-        <v>49722.222222222226</v>
+        <v>50000.000000000044</v>
       </c>
       <c r="C11" s="35">
         <v>1000000</v>
       </c>
       <c r="D11" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="E11" s="41">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="F11" s="36">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G11" s="37" t="str">
         <v>#N/A</v>
@@ -7717,7 +7883,7 @@
         <v>30/360 (Bond Basis)</v>
       </c>
       <c r="K11" s="38">
-        <v>0.99444444444444446</v>
+        <v>1</v>
       </c>
       <c r="L11" s="39">
         <v>0.05</v>
@@ -8920,7 +9086,7 @@
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
@@ -8932,9 +9098,7 @@
     <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.83203125" bestFit="1" customWidth="1"/>
@@ -9009,22 +9173,22 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="34">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="B2" s="35">
-        <v>45644.709190771478</v>
+        <v>46021.587250758144</v>
       </c>
       <c r="C2" s="35">
         <v>1000000</v>
       </c>
       <c r="D2" s="41">
-        <v>41772</v>
+        <v>42103</v>
       </c>
       <c r="E2" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="F2" s="36">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="G2" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9033,16 +9197,16 @@
         <v>2</v>
       </c>
       <c r="I2" s="41">
-        <v>41768</v>
+        <v>42101</v>
       </c>
       <c r="J2" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K2" s="38">
-        <v>1.0138888888888888</v>
+        <v>1.0222222222222221</v>
       </c>
       <c r="L2" s="39">
-        <v>4.5019439201856803E-2</v>
+        <v>4.5021117962698191E-2</v>
       </c>
       <c r="M2" s="39" t="str">
         <v>#N/A</v>
@@ -9051,7 +9215,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="39">
-        <v>4.5019439201856803E-2</v>
+        <v>4.5021117962698191E-2</v>
       </c>
       <c r="P2" s="39">
         <v>0</v>
@@ -9074,22 +9238,22 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="34">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="B3" s="35">
-        <v>45965.940727128131</v>
+        <v>45700.234002910169</v>
       </c>
       <c r="C3" s="35">
         <v>1000000</v>
       </c>
       <c r="D3" s="41">
-        <v>42137</v>
+        <v>42471</v>
       </c>
       <c r="E3" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="F3" s="36">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G3" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9098,16 +9262,16 @@
         <v>2</v>
       </c>
       <c r="I3" s="41">
-        <v>42135</v>
+        <v>42467</v>
       </c>
       <c r="J3" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K3" s="38">
-        <v>1.0166666666666666</v>
+        <v>1.0111111111111111</v>
       </c>
       <c r="L3" s="39">
-        <v>4.5212400715208004E-2</v>
+        <v>4.5198033629251823E-2</v>
       </c>
       <c r="M3" s="39" t="str">
         <v>#N/A</v>
@@ -9116,10 +9280,10 @@
         <v>1</v>
       </c>
       <c r="O3" s="39">
-        <v>4.502110877876498E-2</v>
+        <v>4.5007086676381654E-2</v>
       </c>
       <c r="P3" s="39">
-        <v>1.912919364430235E-4</v>
+        <v>1.9094695287016905E-4</v>
       </c>
       <c r="Q3" s="39">
         <v>0</v>
@@ -9139,22 +9303,22 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="34">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="B4" s="35">
-        <v>46275.038644473956</v>
+        <v>45897.754769535633</v>
       </c>
       <c r="C4" s="35">
         <v>1000000</v>
       </c>
       <c r="D4" s="41">
-        <v>42503</v>
+        <v>42835</v>
       </c>
       <c r="E4" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="F4" s="36">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G4" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9163,16 +9327,16 @@
         <v>2</v>
       </c>
       <c r="I4" s="41">
-        <v>42501</v>
+        <v>42831</v>
       </c>
       <c r="J4" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K4" s="38">
-        <v>1.0194444444444444</v>
+        <v>1.0111111111111111</v>
       </c>
       <c r="L4" s="39">
-        <v>4.5392408479592986E-2</v>
+        <v>4.5393383838002281E-2</v>
       </c>
       <c r="M4" s="39" t="str">
         <v>#N/A</v>
@@ -9181,10 +9345,10 @@
         <v>1</v>
       </c>
       <c r="O4" s="39">
-        <v>4.5006931640100688E-2</v>
+        <v>4.5008215591537871E-2</v>
       </c>
       <c r="P4" s="39">
-        <v>3.8547683949229777E-4</v>
+        <v>3.8516824646440961E-4</v>
       </c>
       <c r="Q4" s="39">
         <v>0</v>
@@ -9204,22 +9368,22 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="34">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="B5" s="35">
-        <v>46100.705678090198</v>
+        <v>46236.176220051486</v>
       </c>
       <c r="C5" s="35">
         <v>1000000</v>
       </c>
       <c r="D5" s="41">
-        <v>42870</v>
+        <v>43199</v>
       </c>
       <c r="E5" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="F5" s="36">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G5" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9228,16 +9392,16 @@
         <v>2</v>
       </c>
       <c r="I5" s="41">
-        <v>42866</v>
+        <v>43195</v>
       </c>
       <c r="J5" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K5" s="38">
-        <v>1.0111111111111111</v>
+        <v>1.0138888888888888</v>
       </c>
       <c r="L5" s="39">
-        <v>4.5594104516792508E-2</v>
+        <v>4.5602803943064485E-2</v>
       </c>
       <c r="M5" s="39" t="str">
         <v>#N/A</v>
@@ -9246,10 +9410,10 @@
         <v>1</v>
       </c>
       <c r="O5" s="39">
-        <v>4.5008179983093845E-2</v>
+        <v>4.5019506828358764E-2</v>
       </c>
       <c r="P5" s="39">
-        <v>5.8592453369866321E-4</v>
+        <v>5.832971147057206E-4</v>
       </c>
       <c r="Q5" s="39">
         <v>0</v>
@@ -9269,22 +9433,22 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="34">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="B6" s="35">
-        <v>46317.59147018251</v>
+        <v>46571.044146595494</v>
       </c>
       <c r="C6" s="35">
         <v>1000000</v>
       </c>
       <c r="D6" s="41">
-        <v>43234</v>
+        <v>43564</v>
       </c>
       <c r="E6" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="F6" s="36">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="G6" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9293,16 +9457,16 @@
         <v>2</v>
       </c>
       <c r="I6" s="41">
-        <v>43230</v>
+        <v>43560</v>
       </c>
       <c r="J6" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K6" s="38">
-        <v>1.0111111111111111</v>
+        <v>1.0166666666666666</v>
       </c>
       <c r="L6" s="39">
-        <v>4.580860694853215E-2</v>
+        <v>4.580758440648737E-2</v>
       </c>
       <c r="M6" s="39" t="str">
         <v>#N/A</v>
@@ -9311,10 +9475,10 @@
         <v>1</v>
       </c>
       <c r="O6" s="39">
-        <v>4.5019502408633533E-2</v>
+        <v>4.5021105506382955E-2</v>
       </c>
       <c r="P6" s="39">
-        <v>7.8910453989861767E-4</v>
+        <v>7.8647890010441479E-4</v>
       </c>
       <c r="Q6" s="39">
         <v>0</v>
@@ -9334,22 +9498,22 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="34">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="B7" s="35">
-        <v>46783.905135645306</v>
+        <v>46641.337224146693</v>
       </c>
       <c r="C7" s="35">
         <v>1000000</v>
       </c>
       <c r="D7" s="41">
-        <v>43598</v>
+        <v>43930</v>
       </c>
       <c r="E7" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="F7" s="36">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G7" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9358,16 +9522,16 @@
         <v>2</v>
       </c>
       <c r="I7" s="41">
-        <v>43594</v>
+        <v>43928</v>
       </c>
       <c r="J7" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K7" s="38">
-        <v>1.0166666666666666</v>
+        <v>1.0138888888888888</v>
       </c>
       <c r="L7" s="39">
-        <v>4.6016955871126537E-2</v>
+        <v>4.6002414796418659E-2</v>
       </c>
       <c r="M7" s="39" t="str">
         <v>#N/A</v>
@@ -9376,10 +9540,10 @@
         <v>1</v>
       </c>
       <c r="O7" s="39">
-        <v>4.502117585177965E-2</v>
+        <v>4.5006928221515731E-2</v>
       </c>
       <c r="P7" s="39">
-        <v>9.9578001934688687E-4</v>
+        <v>9.9548657490292763E-4</v>
       </c>
       <c r="Q7" s="39">
         <v>0</v>
@@ -9399,22 +9563,22 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="B8" s="35">
-        <v>46857.793497313723</v>
+        <v>47112.214357766999</v>
       </c>
       <c r="C8" s="35">
         <v>1000000</v>
       </c>
       <c r="D8" s="41">
-        <v>43964</v>
+        <v>44295</v>
       </c>
       <c r="E8" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="F8" s="36">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G8" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9423,16 +9587,16 @@
         <v>2</v>
       </c>
       <c r="I8" s="41">
-        <v>43962</v>
+        <v>44293</v>
       </c>
       <c r="J8" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K8" s="38">
-        <v>1.0138888888888888</v>
+        <v>1.0194444444444444</v>
       </c>
       <c r="L8" s="39">
-        <v>4.6215905915158749E-2</v>
+        <v>4.6213616263749646E-2</v>
       </c>
       <c r="M8" s="39" t="str">
         <v>#N/A</v>
@@ -9441,10 +9605,10 @@
         <v>1</v>
       </c>
       <c r="O8" s="39">
-        <v>4.5006928165107256E-2</v>
+        <v>4.5008034218931466E-2</v>
       </c>
       <c r="P8" s="39">
-        <v>1.2089777500514931E-3</v>
+        <v>1.2055820448181806E-3</v>
       </c>
       <c r="Q8" s="39">
         <v>0</v>
@@ -9464,19 +9628,19 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="B9" s="35">
-        <v>47078.945134035079</v>
+        <v>47090.565819230549</v>
       </c>
       <c r="C9" s="35">
         <v>1000000</v>
       </c>
       <c r="D9" s="41">
-        <v>44329</v>
+        <v>44662</v>
       </c>
       <c r="E9" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="F9" s="36">
         <v>365</v>
@@ -9488,7 +9652,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="41">
-        <v>44327</v>
+        <v>44658</v>
       </c>
       <c r="J9" s="36" t="str">
         <v>Actual/360</v>
@@ -9497,7 +9661,7 @@
         <v>1.0138888888888888</v>
       </c>
       <c r="L9" s="39">
-        <v>4.643402807740446E-2</v>
+        <v>4.6445489575131504E-2</v>
       </c>
       <c r="M9" s="39" t="str">
         <v>#N/A</v>
@@ -9506,10 +9670,10 @@
         <v>1</v>
       </c>
       <c r="O9" s="39">
-        <v>4.500803415998271E-2</v>
+        <v>4.5019527592106562E-2</v>
       </c>
       <c r="P9" s="39">
-        <v>1.4259939174217501E-3</v>
+        <v>1.4259619830249426E-3</v>
       </c>
       <c r="Q9" s="39">
         <v>0</v>
@@ -9529,22 +9693,22 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="B10" s="35">
-        <v>47572.145779551589</v>
+        <v>47188.95522306973</v>
       </c>
       <c r="C10" s="35">
         <v>1000000</v>
       </c>
       <c r="D10" s="41">
-        <v>44694</v>
+        <v>45027</v>
       </c>
       <c r="E10" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="F10" s="36">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G10" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9553,16 +9717,16 @@
         <v>2</v>
       </c>
       <c r="I10" s="41">
-        <v>44692</v>
+        <v>45021</v>
       </c>
       <c r="J10" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K10" s="38">
-        <v>1.0194444444444444</v>
+        <v>1.0111111111111111</v>
       </c>
       <c r="L10" s="39">
-        <v>4.6664775151603742E-2</v>
+        <v>4.6670395275563471E-2</v>
       </c>
       <c r="M10" s="39" t="str">
         <v>#N/A</v>
@@ -9571,10 +9735,10 @@
         <v>1</v>
       </c>
       <c r="O10" s="39">
-        <v>4.5019441051630464E-2</v>
+        <v>4.5021127210402197E-2</v>
       </c>
       <c r="P10" s="39">
-        <v>1.645334099973278E-3</v>
+        <v>1.6492680651612746E-3</v>
       </c>
       <c r="Q10" s="39">
         <v>0</v>
@@ -9594,22 +9758,22 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="B11" s="35">
-        <v>47421.574501604286</v>
+        <v>47531.46930844945</v>
       </c>
       <c r="C11" s="35">
         <v>1000000</v>
       </c>
       <c r="D11" s="41">
-        <v>45061</v>
+        <v>45391</v>
       </c>
       <c r="E11" s="41">
-        <v>45425</v>
+        <v>45756</v>
       </c>
       <c r="F11" s="36">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G11" s="37" t="str">
         <v>EuriborSwapIsdaFixA10Y 30/360 (Bond Basis)</v>
@@ -9618,16 +9782,16 @@
         <v>2</v>
       </c>
       <c r="I11" s="41">
-        <v>45057</v>
+        <v>45387</v>
       </c>
       <c r="J11" s="36" t="str">
         <v>Actual/360</v>
       </c>
       <c r="K11" s="38">
-        <v>1.0111111111111111</v>
+        <v>1.0138888888888888</v>
       </c>
       <c r="L11" s="39">
-        <v>4.6900458298289954E-2</v>
+        <v>4.6880353290525492E-2</v>
       </c>
       <c r="M11" s="39" t="str">
         <v>#N/A</v>
@@ -9636,10 +9800,10 @@
         <v>1</v>
       </c>
       <c r="O11" s="39">
-        <v>4.5021175851779609E-2</v>
+        <v>4.5007071093443957E-2</v>
       </c>
       <c r="P11" s="39">
-        <v>1.8792824465103455E-3</v>
+        <v>1.8732821970815355E-3</v>
       </c>
       <c r="Q11" s="39">
         <v>0</v>

</xml_diff>